<commit_message>
Added new files for equity calculation
</commit_message>
<xml_diff>
--- a/out/equity/history/INE040H01021-Suzlon Engergy Ltd.xlsx
+++ b/out/equity/history/INE040H01021-Suzlon Engergy Ltd.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M361"/>
+  <dimension ref="A1:M365"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -536,7 +536,7 @@
       <c r="H2" t="n">
         <v>141233544</v>
       </c>
-      <c r="I2" s="3" t="n">
+      <c r="I2" s="2" t="n">
         <v>45518</v>
       </c>
       <c r="J2" t="inlineStr">
@@ -589,7 +589,7 @@
       <c r="H3" t="n">
         <v>154585237</v>
       </c>
-      <c r="I3" s="3" t="n">
+      <c r="I3" s="2" t="n">
         <v>45520</v>
       </c>
       <c r="J3" t="inlineStr">
@@ -642,7 +642,7 @@
       <c r="H4" t="n">
         <v>94333988</v>
       </c>
-      <c r="I4" s="3" t="n">
+      <c r="I4" s="2" t="n">
         <v>45523</v>
       </c>
       <c r="J4" t="inlineStr">
@@ -695,7 +695,7 @@
       <c r="H5" t="n">
         <v>53461818</v>
       </c>
-      <c r="I5" s="3" t="n">
+      <c r="I5" s="2" t="n">
         <v>45524</v>
       </c>
       <c r="J5" t="inlineStr">
@@ -748,7 +748,7 @@
       <c r="H6" t="n">
         <v>38598019</v>
       </c>
-      <c r="I6" s="3" t="n">
+      <c r="I6" s="2" t="n">
         <v>45525</v>
       </c>
       <c r="J6" t="inlineStr">
@@ -801,7 +801,7 @@
       <c r="H7" t="n">
         <v>41304868</v>
       </c>
-      <c r="I7" s="3" t="n">
+      <c r="I7" s="2" t="n">
         <v>45526</v>
       </c>
       <c r="J7" t="inlineStr">
@@ -854,7 +854,7 @@
       <c r="H8" t="n">
         <v>67099843</v>
       </c>
-      <c r="I8" s="3" t="n">
+      <c r="I8" s="2" t="n">
         <v>45527</v>
       </c>
       <c r="J8" t="inlineStr">
@@ -907,7 +907,7 @@
       <c r="H9" t="n">
         <v>57530895</v>
       </c>
-      <c r="I9" s="3" t="n">
+      <c r="I9" s="2" t="n">
         <v>45530</v>
       </c>
       <c r="J9" t="inlineStr">
@@ -960,7 +960,7 @@
       <c r="H10" t="n">
         <v>32345582</v>
       </c>
-      <c r="I10" s="3" t="n">
+      <c r="I10" s="2" t="n">
         <v>45531</v>
       </c>
       <c r="J10" t="inlineStr">
@@ -1013,7 +1013,7 @@
       <c r="H11" t="n">
         <v>47504013</v>
       </c>
-      <c r="I11" s="3" t="n">
+      <c r="I11" s="2" t="n">
         <v>45532</v>
       </c>
       <c r="J11" t="inlineStr">
@@ -1066,7 +1066,7 @@
       <c r="H12" t="n">
         <v>41667115</v>
       </c>
-      <c r="I12" s="3" t="n">
+      <c r="I12" s="2" t="n">
         <v>45533</v>
       </c>
       <c r="J12" t="inlineStr">
@@ -1119,7 +1119,7 @@
       <c r="H13" t="n">
         <v>63629231</v>
       </c>
-      <c r="I13" s="3" t="n">
+      <c r="I13" s="2" t="n">
         <v>45534</v>
       </c>
       <c r="J13" t="inlineStr">
@@ -1172,7 +1172,7 @@
       <c r="H14" t="n">
         <v>71527116</v>
       </c>
-      <c r="I14" s="3" t="n">
+      <c r="I14" s="2" t="n">
         <v>45537</v>
       </c>
       <c r="J14" t="inlineStr">
@@ -1225,7 +1225,7 @@
       <c r="H15" t="n">
         <v>49100490</v>
       </c>
-      <c r="I15" s="3" t="n">
+      <c r="I15" s="2" t="n">
         <v>45538</v>
       </c>
       <c r="J15" t="inlineStr">
@@ -1278,7 +1278,7 @@
       <c r="H16" t="n">
         <v>28105608</v>
       </c>
-      <c r="I16" s="3" t="n">
+      <c r="I16" s="2" t="n">
         <v>45539</v>
       </c>
       <c r="J16" t="inlineStr">
@@ -1331,7 +1331,7 @@
       <c r="H17" t="n">
         <v>55889917</v>
       </c>
-      <c r="I17" s="3" t="n">
+      <c r="I17" s="2" t="n">
         <v>45540</v>
       </c>
       <c r="J17" t="inlineStr">
@@ -1384,7 +1384,7 @@
       <c r="H18" t="n">
         <v>43160865</v>
       </c>
-      <c r="I18" s="3" t="n">
+      <c r="I18" s="2" t="n">
         <v>45541</v>
       </c>
       <c r="J18" t="inlineStr">
@@ -1437,7 +1437,7 @@
       <c r="H19" t="n">
         <v>86932752</v>
       </c>
-      <c r="I19" s="3" t="n">
+      <c r="I19" s="2" t="n">
         <v>45544</v>
       </c>
       <c r="J19" t="inlineStr">
@@ -1490,7 +1490,7 @@
       <c r="H20" t="n">
         <v>144050217</v>
       </c>
-      <c r="I20" s="3" t="n">
+      <c r="I20" s="2" t="n">
         <v>45545</v>
       </c>
       <c r="J20" t="inlineStr">
@@ -1543,7 +1543,7 @@
       <c r="H21" t="n">
         <v>118203835</v>
       </c>
-      <c r="I21" s="3" t="n">
+      <c r="I21" s="2" t="n">
         <v>45546</v>
       </c>
       <c r="J21" t="inlineStr">
@@ -1596,7 +1596,7 @@
       <c r="H22" t="n">
         <v>175874631</v>
       </c>
-      <c r="I22" s="3" t="n">
+      <c r="I22" s="2" t="n">
         <v>45547</v>
       </c>
       <c r="J22" t="inlineStr">
@@ -1649,7 +1649,7 @@
       <c r="H23" t="n">
         <v>82231123</v>
       </c>
-      <c r="I23" s="3" t="n">
+      <c r="I23" s="2" t="n">
         <v>45548</v>
       </c>
       <c r="J23" t="inlineStr">
@@ -1702,7 +1702,7 @@
       <c r="H24" t="n">
         <v>67330344</v>
       </c>
-      <c r="I24" s="3" t="n">
+      <c r="I24" s="2" t="n">
         <v>45551</v>
       </c>
       <c r="J24" t="inlineStr">
@@ -1755,7 +1755,7 @@
       <c r="H25" t="n">
         <v>60635579</v>
       </c>
-      <c r="I25" s="3" t="n">
+      <c r="I25" s="2" t="n">
         <v>45552</v>
       </c>
       <c r="J25" t="inlineStr">
@@ -1808,7 +1808,7 @@
       <c r="H26" t="n">
         <v>37365891</v>
       </c>
-      <c r="I26" s="3" t="n">
+      <c r="I26" s="2" t="n">
         <v>45553</v>
       </c>
       <c r="J26" t="inlineStr">
@@ -1861,7 +1861,7 @@
       <c r="H27" t="n">
         <v>60208144</v>
       </c>
-      <c r="I27" s="3" t="n">
+      <c r="I27" s="2" t="n">
         <v>45554</v>
       </c>
       <c r="J27" t="inlineStr">
@@ -1914,7 +1914,7 @@
       <c r="H28" t="n">
         <v>73831742</v>
       </c>
-      <c r="I28" s="3" t="n">
+      <c r="I28" s="2" t="n">
         <v>45555</v>
       </c>
       <c r="J28" t="inlineStr">
@@ -1967,7 +1967,7 @@
       <c r="H29" t="n">
         <v>34830182</v>
       </c>
-      <c r="I29" s="3" t="n">
+      <c r="I29" s="2" t="n">
         <v>45558</v>
       </c>
       <c r="J29" t="inlineStr">
@@ -2020,7 +2020,7 @@
       <c r="H30" t="n">
         <v>34171361</v>
       </c>
-      <c r="I30" s="3" t="n">
+      <c r="I30" s="2" t="n">
         <v>45559</v>
       </c>
       <c r="J30" t="inlineStr">
@@ -2073,7 +2073,7 @@
       <c r="H31" t="n">
         <v>26723081</v>
       </c>
-      <c r="I31" s="3" t="n">
+      <c r="I31" s="2" t="n">
         <v>45560</v>
       </c>
       <c r="J31" t="inlineStr">
@@ -2126,7 +2126,7 @@
       <c r="H32" t="n">
         <v>24765918</v>
       </c>
-      <c r="I32" s="3" t="n">
+      <c r="I32" s="2" t="n">
         <v>45561</v>
       </c>
       <c r="J32" t="inlineStr">
@@ -2179,7 +2179,7 @@
       <c r="H33" t="n">
         <v>42391607</v>
       </c>
-      <c r="I33" s="3" t="n">
+      <c r="I33" s="2" t="n">
         <v>45562</v>
       </c>
       <c r="J33" t="inlineStr">
@@ -2232,7 +2232,7 @@
       <c r="H34" t="n">
         <v>42014699</v>
       </c>
-      <c r="I34" s="3" t="n">
+      <c r="I34" s="2" t="n">
         <v>45565</v>
       </c>
       <c r="J34" t="inlineStr">
@@ -2285,7 +2285,7 @@
       <c r="H35" t="n">
         <v>27355780</v>
       </c>
-      <c r="I35" s="3" t="n">
+      <c r="I35" s="2" t="n">
         <v>45566</v>
       </c>
       <c r="J35" t="inlineStr">
@@ -2338,7 +2338,7 @@
       <c r="H36" t="n">
         <v>78969350</v>
       </c>
-      <c r="I36" s="3" t="n">
+      <c r="I36" s="2" t="n">
         <v>45568</v>
       </c>
       <c r="J36" t="inlineStr">
@@ -2391,7 +2391,7 @@
       <c r="H37" t="n">
         <v>77532421</v>
       </c>
-      <c r="I37" s="3" t="n">
+      <c r="I37" s="2" t="n">
         <v>45569</v>
       </c>
       <c r="J37" t="inlineStr">
@@ -2444,7 +2444,7 @@
       <c r="H38" t="n">
         <v>76418591</v>
       </c>
-      <c r="I38" s="3" t="n">
+      <c r="I38" s="2" t="n">
         <v>45572</v>
       </c>
       <c r="J38" t="inlineStr">
@@ -2497,7 +2497,7 @@
       <c r="H39" t="n">
         <v>134136634</v>
       </c>
-      <c r="I39" s="3" t="n">
+      <c r="I39" s="2" t="n">
         <v>45573</v>
       </c>
       <c r="J39" t="inlineStr">
@@ -2550,7 +2550,7 @@
       <c r="H40" t="n">
         <v>135423689</v>
       </c>
-      <c r="I40" s="3" t="n">
+      <c r="I40" s="2" t="n">
         <v>45574</v>
       </c>
       <c r="J40" t="inlineStr">
@@ -2603,7 +2603,7 @@
       <c r="H41" t="n">
         <v>70279343</v>
       </c>
-      <c r="I41" s="3" t="n">
+      <c r="I41" s="2" t="n">
         <v>45575</v>
       </c>
       <c r="J41" t="inlineStr">
@@ -2656,7 +2656,7 @@
       <c r="H42" t="n">
         <v>32439764</v>
       </c>
-      <c r="I42" s="3" t="n">
+      <c r="I42" s="2" t="n">
         <v>45576</v>
       </c>
       <c r="J42" t="inlineStr">
@@ -2709,7 +2709,7 @@
       <c r="H43" t="n">
         <v>24788829</v>
       </c>
-      <c r="I43" s="3" t="n">
+      <c r="I43" s="2" t="n">
         <v>45579</v>
       </c>
       <c r="J43" t="inlineStr">
@@ -2762,7 +2762,7 @@
       <c r="H44" t="n">
         <v>42286299</v>
       </c>
-      <c r="I44" s="3" t="n">
+      <c r="I44" s="2" t="n">
         <v>45580</v>
       </c>
       <c r="J44" t="inlineStr">
@@ -2815,7 +2815,7 @@
       <c r="H45" t="n">
         <v>46739056</v>
       </c>
-      <c r="I45" s="3" t="n">
+      <c r="I45" s="2" t="n">
         <v>45581</v>
       </c>
       <c r="J45" t="inlineStr">
@@ -2868,7 +2868,7 @@
       <c r="H46" t="n">
         <v>32018973</v>
       </c>
-      <c r="I46" s="3" t="n">
+      <c r="I46" s="2" t="n">
         <v>45582</v>
       </c>
       <c r="J46" t="inlineStr">
@@ -2921,7 +2921,7 @@
       <c r="H47" t="n">
         <v>35817127</v>
       </c>
-      <c r="I47" s="3" t="n">
+      <c r="I47" s="2" t="n">
         <v>45583</v>
       </c>
       <c r="J47" t="inlineStr">
@@ -2974,7 +2974,7 @@
       <c r="H48" t="n">
         <v>26801015</v>
       </c>
-      <c r="I48" s="3" t="n">
+      <c r="I48" s="2" t="n">
         <v>45586</v>
       </c>
       <c r="J48" t="inlineStr">
@@ -3027,7 +3027,7 @@
       <c r="H49" t="n">
         <v>67520436</v>
       </c>
-      <c r="I49" s="3" t="n">
+      <c r="I49" s="2" t="n">
         <v>45587</v>
       </c>
       <c r="J49" t="inlineStr">
@@ -3080,7 +3080,7 @@
       <c r="H50" t="n">
         <v>54998823</v>
       </c>
-      <c r="I50" s="3" t="n">
+      <c r="I50" s="2" t="n">
         <v>45588</v>
       </c>
       <c r="J50" t="inlineStr">
@@ -3133,7 +3133,7 @@
       <c r="H51" t="n">
         <v>34935271</v>
       </c>
-      <c r="I51" s="3" t="n">
+      <c r="I51" s="2" t="n">
         <v>45589</v>
       </c>
       <c r="J51" t="inlineStr">
@@ -3186,7 +3186,7 @@
       <c r="H52" t="n">
         <v>49200584</v>
       </c>
-      <c r="I52" s="3" t="n">
+      <c r="I52" s="2" t="n">
         <v>45590</v>
       </c>
       <c r="J52" t="inlineStr">
@@ -3239,7 +3239,7 @@
       <c r="H53" t="n">
         <v>81565524</v>
       </c>
-      <c r="I53" s="3" t="n">
+      <c r="I53" s="2" t="n">
         <v>45593</v>
       </c>
       <c r="J53" t="inlineStr">
@@ -3292,7 +3292,7 @@
       <c r="H54" t="n">
         <v>128660437</v>
       </c>
-      <c r="I54" s="3" t="n">
+      <c r="I54" s="2" t="n">
         <v>45594</v>
       </c>
       <c r="J54" t="inlineStr">
@@ -3345,7 +3345,7 @@
       <c r="H55" t="n">
         <v>52550622</v>
       </c>
-      <c r="I55" s="3" t="n">
+      <c r="I55" s="2" t="n">
         <v>45595</v>
       </c>
       <c r="J55" t="inlineStr">
@@ -3398,7 +3398,7 @@
       <c r="H56" t="n">
         <v>41205444</v>
       </c>
-      <c r="I56" s="3" t="n">
+      <c r="I56" s="2" t="n">
         <v>45596</v>
       </c>
       <c r="J56" t="inlineStr">
@@ -3451,7 +3451,7 @@
       <c r="H57" t="n">
         <v>11638197</v>
       </c>
-      <c r="I57" s="3" t="n">
+      <c r="I57" s="2" t="n">
         <v>45597</v>
       </c>
       <c r="J57" t="inlineStr">
@@ -3504,7 +3504,7 @@
       <c r="H58" t="n">
         <v>55155511</v>
       </c>
-      <c r="I58" s="3" t="n">
+      <c r="I58" s="2" t="n">
         <v>45600</v>
       </c>
       <c r="J58" t="inlineStr">
@@ -3557,7 +3557,7 @@
       <c r="H59" t="n">
         <v>45455406</v>
       </c>
-      <c r="I59" s="3" t="n">
+      <c r="I59" s="2" t="n">
         <v>45601</v>
       </c>
       <c r="J59" t="inlineStr">
@@ -3610,7 +3610,7 @@
       <c r="H60" t="n">
         <v>49820172</v>
       </c>
-      <c r="I60" s="3" t="n">
+      <c r="I60" s="2" t="n">
         <v>45602</v>
       </c>
       <c r="J60" t="inlineStr">
@@ -3663,7 +3663,7 @@
       <c r="H61" t="n">
         <v>49042798</v>
       </c>
-      <c r="I61" s="3" t="n">
+      <c r="I61" s="2" t="n">
         <v>45603</v>
       </c>
       <c r="J61" t="inlineStr">
@@ -3716,7 +3716,7 @@
       <c r="H62" t="n">
         <v>85921733</v>
       </c>
-      <c r="I62" s="3" t="n">
+      <c r="I62" s="2" t="n">
         <v>45604</v>
       </c>
       <c r="J62" t="inlineStr">
@@ -3769,7 +3769,7 @@
       <c r="H63" t="n">
         <v>127626529</v>
       </c>
-      <c r="I63" s="3" t="n">
+      <c r="I63" s="2" t="n">
         <v>45607</v>
       </c>
       <c r="J63" t="inlineStr">
@@ -3822,7 +3822,7 @@
       <c r="H64" t="n">
         <v>67412418</v>
       </c>
-      <c r="I64" s="3" t="n">
+      <c r="I64" s="2" t="n">
         <v>45608</v>
       </c>
       <c r="J64" t="inlineStr">
@@ -3875,7 +3875,7 @@
       <c r="H65" t="n">
         <v>193740055</v>
       </c>
-      <c r="I65" s="3" t="n">
+      <c r="I65" s="2" t="n">
         <v>45609</v>
       </c>
       <c r="J65" t="inlineStr">
@@ -3928,7 +3928,7 @@
       <c r="H66" t="n">
         <v>56285831</v>
       </c>
-      <c r="I66" s="3" t="n">
+      <c r="I66" s="2" t="n">
         <v>45610</v>
       </c>
       <c r="J66" t="inlineStr">
@@ -3981,7 +3981,7 @@
       <c r="H67" t="n">
         <v>114646213</v>
       </c>
-      <c r="I67" s="3" t="n">
+      <c r="I67" s="2" t="n">
         <v>45614</v>
       </c>
       <c r="J67" t="inlineStr">
@@ -4034,7 +4034,7 @@
       <c r="H68" t="n">
         <v>72025938</v>
       </c>
-      <c r="I68" s="3" t="n">
+      <c r="I68" s="2" t="n">
         <v>45615</v>
       </c>
       <c r="J68" t="inlineStr">
@@ -4087,7 +4087,7 @@
       <c r="H69" t="n">
         <v>129063640</v>
       </c>
-      <c r="I69" s="3" t="n">
+      <c r="I69" s="2" t="n">
         <v>45617</v>
       </c>
       <c r="J69" t="inlineStr">
@@ -4140,7 +4140,7 @@
       <c r="H70" t="n">
         <v>128624960</v>
       </c>
-      <c r="I70" s="3" t="n">
+      <c r="I70" s="2" t="n">
         <v>45618</v>
       </c>
       <c r="J70" t="inlineStr">
@@ -4193,7 +4193,7 @@
       <c r="H71" t="n">
         <v>122951304</v>
       </c>
-      <c r="I71" s="3" t="n">
+      <c r="I71" s="2" t="n">
         <v>45621</v>
       </c>
       <c r="J71" t="inlineStr">
@@ -4246,7 +4246,7 @@
       <c r="H72" t="n">
         <v>35093877</v>
       </c>
-      <c r="I72" s="3" t="n">
+      <c r="I72" s="2" t="n">
         <v>45622</v>
       </c>
       <c r="J72" t="inlineStr">
@@ -4299,7 +4299,7 @@
       <c r="H73" t="n">
         <v>37010704</v>
       </c>
-      <c r="I73" s="3" t="n">
+      <c r="I73" s="2" t="n">
         <v>45623</v>
       </c>
       <c r="J73" t="inlineStr">
@@ -4352,7 +4352,7 @@
       <c r="H74" t="n">
         <v>42327418</v>
       </c>
-      <c r="I74" s="3" t="n">
+      <c r="I74" s="2" t="n">
         <v>45624</v>
       </c>
       <c r="J74" t="inlineStr">
@@ -4405,7 +4405,7 @@
       <c r="H75" t="n">
         <v>54611932</v>
       </c>
-      <c r="I75" s="3" t="n">
+      <c r="I75" s="2" t="n">
         <v>45625</v>
       </c>
       <c r="J75" t="inlineStr">
@@ -4458,7 +4458,7 @@
       <c r="H76" t="n">
         <v>60811076</v>
       </c>
-      <c r="I76" s="3" t="n">
+      <c r="I76" s="2" t="n">
         <v>45628</v>
       </c>
       <c r="J76" t="inlineStr">
@@ -4511,7 +4511,7 @@
       <c r="H77" t="n">
         <v>87567298</v>
       </c>
-      <c r="I77" s="3" t="n">
+      <c r="I77" s="2" t="n">
         <v>45629</v>
       </c>
       <c r="J77" t="inlineStr">
@@ -4564,7 +4564,7 @@
       <c r="H78" t="n">
         <v>97274583</v>
       </c>
-      <c r="I78" s="3" t="n">
+      <c r="I78" s="2" t="n">
         <v>45630</v>
       </c>
       <c r="J78" t="inlineStr">
@@ -4617,7 +4617,7 @@
       <c r="H79" t="n">
         <v>55819076</v>
       </c>
-      <c r="I79" s="3" t="n">
+      <c r="I79" s="2" t="n">
         <v>45631</v>
       </c>
       <c r="J79" t="inlineStr">
@@ -4670,7 +4670,7 @@
       <c r="H80" t="n">
         <v>37879441</v>
       </c>
-      <c r="I80" s="3" t="n">
+      <c r="I80" s="2" t="n">
         <v>45632</v>
       </c>
       <c r="J80" t="inlineStr">
@@ -4723,7 +4723,7 @@
       <c r="H81" t="n">
         <v>34265183</v>
       </c>
-      <c r="I81" s="3" t="n">
+      <c r="I81" s="2" t="n">
         <v>45635</v>
       </c>
       <c r="J81" t="inlineStr">
@@ -4776,7 +4776,7 @@
       <c r="H82" t="n">
         <v>29422592</v>
       </c>
-      <c r="I82" s="3" t="n">
+      <c r="I82" s="2" t="n">
         <v>45636</v>
       </c>
       <c r="J82" t="inlineStr">
@@ -4829,7 +4829,7 @@
       <c r="H83" t="n">
         <v>32364680</v>
       </c>
-      <c r="I83" s="3" t="n">
+      <c r="I83" s="2" t="n">
         <v>45637</v>
       </c>
       <c r="J83" t="inlineStr">
@@ -4882,7 +4882,7 @@
       <c r="H84" t="n">
         <v>33411886</v>
       </c>
-      <c r="I84" s="3" t="n">
+      <c r="I84" s="2" t="n">
         <v>45638</v>
       </c>
       <c r="J84" t="inlineStr">
@@ -4935,7 +4935,7 @@
       <c r="H85" t="n">
         <v>47823899</v>
       </c>
-      <c r="I85" s="3" t="n">
+      <c r="I85" s="2" t="n">
         <v>45639</v>
       </c>
       <c r="J85" t="inlineStr">
@@ -4988,7 +4988,7 @@
       <c r="H86" t="n">
         <v>55975666</v>
       </c>
-      <c r="I86" s="3" t="n">
+      <c r="I86" s="2" t="n">
         <v>45642</v>
       </c>
       <c r="J86" t="inlineStr">
@@ -5041,7 +5041,7 @@
       <c r="H87" t="n">
         <v>188130016</v>
       </c>
-      <c r="I87" s="3" t="n">
+      <c r="I87" s="2" t="n">
         <v>45643</v>
       </c>
       <c r="J87" t="inlineStr">
@@ -5094,7 +5094,7 @@
       <c r="H88" t="n">
         <v>68021121</v>
       </c>
-      <c r="I88" s="3" t="n">
+      <c r="I88" s="2" t="n">
         <v>45644</v>
       </c>
       <c r="J88" t="inlineStr">
@@ -5147,7 +5147,7 @@
       <c r="H89" t="n">
         <v>55271478</v>
       </c>
-      <c r="I89" s="3" t="n">
+      <c r="I89" s="2" t="n">
         <v>45645</v>
       </c>
       <c r="J89" t="inlineStr">
@@ -5200,7 +5200,7 @@
       <c r="H90" t="n">
         <v>54797843</v>
       </c>
-      <c r="I90" s="3" t="n">
+      <c r="I90" s="2" t="n">
         <v>45646</v>
       </c>
       <c r="J90" t="inlineStr">
@@ -5253,7 +5253,7 @@
       <c r="H91" t="n">
         <v>29689351</v>
       </c>
-      <c r="I91" s="3" t="n">
+      <c r="I91" s="2" t="n">
         <v>45649</v>
       </c>
       <c r="J91" t="inlineStr">
@@ -5306,7 +5306,7 @@
       <c r="H92" t="n">
         <v>24682959</v>
       </c>
-      <c r="I92" s="3" t="n">
+      <c r="I92" s="2" t="n">
         <v>45650</v>
       </c>
       <c r="J92" t="inlineStr">
@@ -5359,7 +5359,7 @@
       <c r="H93" t="n">
         <v>19394620</v>
       </c>
-      <c r="I93" s="3" t="n">
+      <c r="I93" s="2" t="n">
         <v>45652</v>
       </c>
       <c r="J93" t="inlineStr">
@@ -5412,7 +5412,7 @@
       <c r="H94" t="n">
         <v>20549383</v>
       </c>
-      <c r="I94" s="3" t="n">
+      <c r="I94" s="2" t="n">
         <v>45653</v>
       </c>
       <c r="J94" t="inlineStr">
@@ -5465,7 +5465,7 @@
       <c r="H95" t="n">
         <v>49471858</v>
       </c>
-      <c r="I95" s="3" t="n">
+      <c r="I95" s="2" t="n">
         <v>45656</v>
       </c>
       <c r="J95" t="inlineStr">
@@ -5518,7 +5518,7 @@
       <c r="H96" t="n">
         <v>34748153</v>
       </c>
-      <c r="I96" s="3" t="n">
+      <c r="I96" s="2" t="n">
         <v>45657</v>
       </c>
       <c r="J96" t="inlineStr">
@@ -5571,7 +5571,7 @@
       <c r="H97" t="n">
         <v>62119717</v>
       </c>
-      <c r="I97" s="3" t="n">
+      <c r="I97" s="2" t="n">
         <v>45658</v>
       </c>
       <c r="J97" t="inlineStr">
@@ -5624,7 +5624,7 @@
       <c r="H98" t="n">
         <v>67266639</v>
       </c>
-      <c r="I98" s="3" t="n">
+      <c r="I98" s="2" t="n">
         <v>45659</v>
       </c>
       <c r="J98" t="inlineStr">
@@ -5677,7 +5677,7 @@
       <c r="H99" t="n">
         <v>42439583</v>
       </c>
-      <c r="I99" s="3" t="n">
+      <c r="I99" s="2" t="n">
         <v>45660</v>
       </c>
       <c r="J99" t="inlineStr">
@@ -5730,7 +5730,7 @@
       <c r="H100" t="n">
         <v>62103375</v>
       </c>
-      <c r="I100" s="3" t="n">
+      <c r="I100" s="2" t="n">
         <v>45663</v>
       </c>
       <c r="J100" t="inlineStr">
@@ -5783,7 +5783,7 @@
       <c r="H101" t="n">
         <v>58506127</v>
       </c>
-      <c r="I101" s="3" t="n">
+      <c r="I101" s="2" t="n">
         <v>45664</v>
       </c>
       <c r="J101" t="inlineStr">
@@ -5836,7 +5836,7 @@
       <c r="H102" t="n">
         <v>36957596</v>
       </c>
-      <c r="I102" s="3" t="n">
+      <c r="I102" s="2" t="n">
         <v>45665</v>
       </c>
       <c r="J102" t="inlineStr">
@@ -5889,7 +5889,7 @@
       <c r="H103" t="n">
         <v>34927530</v>
       </c>
-      <c r="I103" s="3" t="n">
+      <c r="I103" s="2" t="n">
         <v>45666</v>
       </c>
       <c r="J103" t="inlineStr">
@@ -5942,7 +5942,7 @@
       <c r="H104" t="n">
         <v>64132266</v>
       </c>
-      <c r="I104" s="3" t="n">
+      <c r="I104" s="2" t="n">
         <v>45667</v>
       </c>
       <c r="J104" t="inlineStr">
@@ -5995,7 +5995,7 @@
       <c r="H105" t="n">
         <v>91646453</v>
       </c>
-      <c r="I105" s="3" t="n">
+      <c r="I105" s="2" t="n">
         <v>45670</v>
       </c>
       <c r="J105" t="inlineStr">
@@ -6048,7 +6048,7 @@
       <c r="H106" t="n">
         <v>40765242</v>
       </c>
-      <c r="I106" s="3" t="n">
+      <c r="I106" s="2" t="n">
         <v>45671</v>
       </c>
       <c r="J106" t="inlineStr">
@@ -6101,7 +6101,7 @@
       <c r="H107" t="n">
         <v>64202160</v>
       </c>
-      <c r="I107" s="3" t="n">
+      <c r="I107" s="2" t="n">
         <v>45672</v>
       </c>
       <c r="J107" t="inlineStr">
@@ -6154,7 +6154,7 @@
       <c r="H108" t="n">
         <v>39627715</v>
       </c>
-      <c r="I108" s="3" t="n">
+      <c r="I108" s="2" t="n">
         <v>45673</v>
       </c>
       <c r="J108" t="inlineStr">
@@ -6207,7 +6207,7 @@
       <c r="H109" t="n">
         <v>41677119</v>
       </c>
-      <c r="I109" s="3" t="n">
+      <c r="I109" s="2" t="n">
         <v>45674</v>
       </c>
       <c r="J109" t="inlineStr">
@@ -6260,7 +6260,7 @@
       <c r="H110" t="n">
         <v>49378726</v>
       </c>
-      <c r="I110" s="3" t="n">
+      <c r="I110" s="2" t="n">
         <v>45677</v>
       </c>
       <c r="J110" t="inlineStr">
@@ -6313,7 +6313,7 @@
       <c r="H111" t="n">
         <v>33851218</v>
       </c>
-      <c r="I111" s="3" t="n">
+      <c r="I111" s="2" t="n">
         <v>45678</v>
       </c>
       <c r="J111" t="inlineStr">
@@ -6366,7 +6366,7 @@
       <c r="H112" t="n">
         <v>48845984</v>
       </c>
-      <c r="I112" s="3" t="n">
+      <c r="I112" s="2" t="n">
         <v>45679</v>
       </c>
       <c r="J112" t="inlineStr">
@@ -6419,7 +6419,7 @@
       <c r="H113" t="n">
         <v>49444016</v>
       </c>
-      <c r="I113" s="3" t="n">
+      <c r="I113" s="2" t="n">
         <v>45680</v>
       </c>
       <c r="J113" t="inlineStr">
@@ -6472,7 +6472,7 @@
       <c r="H114" t="n">
         <v>63598263</v>
       </c>
-      <c r="I114" s="3" t="n">
+      <c r="I114" s="2" t="n">
         <v>45681</v>
       </c>
       <c r="J114" t="inlineStr">
@@ -6525,7 +6525,7 @@
       <c r="H115" t="n">
         <v>65728343</v>
       </c>
-      <c r="I115" s="3" t="n">
+      <c r="I115" s="2" t="n">
         <v>45684</v>
       </c>
       <c r="J115" t="inlineStr">
@@ -6578,7 +6578,7 @@
       <c r="H116" t="n">
         <v>86329952</v>
       </c>
-      <c r="I116" s="3" t="n">
+      <c r="I116" s="2" t="n">
         <v>45685</v>
       </c>
       <c r="J116" t="inlineStr">
@@ -6631,7 +6631,7 @@
       <c r="H117" t="n">
         <v>13294566</v>
       </c>
-      <c r="I117" s="3" t="n">
+      <c r="I117" s="2" t="n">
         <v>45686</v>
       </c>
       <c r="J117" t="inlineStr">
@@ -6684,7 +6684,7 @@
       <c r="H118" t="n">
         <v>10304014</v>
       </c>
-      <c r="I118" s="3" t="n">
+      <c r="I118" s="2" t="n">
         <v>45687</v>
       </c>
       <c r="J118" t="inlineStr">
@@ -6737,7 +6737,7 @@
       <c r="H119" t="n">
         <v>99062016</v>
       </c>
-      <c r="I119" s="3" t="n">
+      <c r="I119" s="2" t="n">
         <v>45688</v>
       </c>
       <c r="J119" t="inlineStr">
@@ -6790,7 +6790,7 @@
       <c r="H120" t="n">
         <v>166757171</v>
       </c>
-      <c r="I120" s="3" t="n">
+      <c r="I120" s="2" t="n">
         <v>45689</v>
       </c>
       <c r="J120" t="inlineStr">
@@ -6843,7 +6843,7 @@
       <c r="H121" t="n">
         <v>92932081</v>
       </c>
-      <c r="I121" s="3" t="n">
+      <c r="I121" s="2" t="n">
         <v>45691</v>
       </c>
       <c r="J121" t="inlineStr">
@@ -6896,7 +6896,7 @@
       <c r="H122" t="n">
         <v>42035336</v>
       </c>
-      <c r="I122" s="3" t="n">
+      <c r="I122" s="2" t="n">
         <v>45692</v>
       </c>
       <c r="J122" t="inlineStr">
@@ -6949,7 +6949,7 @@
       <c r="H123" t="n">
         <v>37666320</v>
       </c>
-      <c r="I123" s="3" t="n">
+      <c r="I123" s="2" t="n">
         <v>45693</v>
       </c>
       <c r="J123" t="inlineStr">
@@ -7002,7 +7002,7 @@
       <c r="H124" t="n">
         <v>31351447</v>
       </c>
-      <c r="I124" s="3" t="n">
+      <c r="I124" s="2" t="n">
         <v>45694</v>
       </c>
       <c r="J124" t="inlineStr">
@@ -7055,7 +7055,7 @@
       <c r="H125" t="n">
         <v>38671284</v>
       </c>
-      <c r="I125" s="3" t="n">
+      <c r="I125" s="2" t="n">
         <v>45695</v>
       </c>
       <c r="J125" t="inlineStr">
@@ -7108,7 +7108,7 @@
       <c r="H126" t="n">
         <v>30913138</v>
       </c>
-      <c r="I126" s="3" t="n">
+      <c r="I126" s="2" t="n">
         <v>45698</v>
       </c>
       <c r="J126" t="inlineStr">
@@ -7161,7 +7161,7 @@
       <c r="H127" t="n">
         <v>49304394</v>
       </c>
-      <c r="I127" s="3" t="n">
+      <c r="I127" s="2" t="n">
         <v>45699</v>
       </c>
       <c r="J127" t="inlineStr">
@@ -7214,7 +7214,7 @@
       <c r="H128" t="n">
         <v>69039346</v>
       </c>
-      <c r="I128" s="3" t="n">
+      <c r="I128" s="2" t="n">
         <v>45700</v>
       </c>
       <c r="J128" t="inlineStr">
@@ -7267,7 +7267,7 @@
       <c r="H129" t="n">
         <v>41431171</v>
       </c>
-      <c r="I129" s="3" t="n">
+      <c r="I129" s="2" t="n">
         <v>45701</v>
       </c>
       <c r="J129" t="inlineStr">
@@ -7320,7 +7320,7 @@
       <c r="H130" t="n">
         <v>45767569</v>
       </c>
-      <c r="I130" s="3" t="n">
+      <c r="I130" s="2" t="n">
         <v>45702</v>
       </c>
       <c r="J130" t="inlineStr">
@@ -7373,7 +7373,7 @@
       <c r="H131" t="n">
         <v>46544572</v>
       </c>
-      <c r="I131" s="3" t="n">
+      <c r="I131" s="2" t="n">
         <v>45705</v>
       </c>
       <c r="J131" t="inlineStr">
@@ -7426,7 +7426,7 @@
       <c r="H132" t="n">
         <v>38793730</v>
       </c>
-      <c r="I132" s="3" t="n">
+      <c r="I132" s="2" t="n">
         <v>45706</v>
       </c>
       <c r="J132" t="inlineStr">
@@ -7479,7 +7479,7 @@
       <c r="H133" t="n">
         <v>71873369</v>
       </c>
-      <c r="I133" s="3" t="n">
+      <c r="I133" s="2" t="n">
         <v>45707</v>
       </c>
       <c r="J133" t="inlineStr">
@@ -7532,7 +7532,7 @@
       <c r="H134" t="n">
         <v>38637801</v>
       </c>
-      <c r="I134" s="3" t="n">
+      <c r="I134" s="2" t="n">
         <v>45708</v>
       </c>
       <c r="J134" t="inlineStr">
@@ -7585,7 +7585,7 @@
       <c r="H135" t="n">
         <v>56552070</v>
       </c>
-      <c r="I135" s="3" t="n">
+      <c r="I135" s="2" t="n">
         <v>45709</v>
       </c>
       <c r="J135" t="inlineStr">
@@ -7638,7 +7638,7 @@
       <c r="H136" t="n">
         <v>42938535</v>
       </c>
-      <c r="I136" s="3" t="n">
+      <c r="I136" s="2" t="n">
         <v>45712</v>
       </c>
       <c r="J136" t="inlineStr">
@@ -7691,7 +7691,7 @@
       <c r="H137" t="n">
         <v>21705737</v>
       </c>
-      <c r="I137" s="3" t="n">
+      <c r="I137" s="2" t="n">
         <v>45713</v>
       </c>
       <c r="J137" t="inlineStr">
@@ -7744,7 +7744,7 @@
       <c r="H138" t="n">
         <v>38792894</v>
       </c>
-      <c r="I138" s="3" t="n">
+      <c r="I138" s="2" t="n">
         <v>45715</v>
       </c>
       <c r="J138" t="inlineStr">
@@ -7797,7 +7797,7 @@
       <c r="H139" t="n">
         <v>92951783</v>
       </c>
-      <c r="I139" s="3" t="n">
+      <c r="I139" s="2" t="n">
         <v>45716</v>
       </c>
       <c r="J139" t="inlineStr">
@@ -7850,7 +7850,7 @@
       <c r="H140" t="n">
         <v>108295994</v>
       </c>
-      <c r="I140" s="3" t="n">
+      <c r="I140" s="2" t="n">
         <v>45719</v>
       </c>
       <c r="J140" t="inlineStr">
@@ -7903,7 +7903,7 @@
       <c r="H141" t="n">
         <v>67369885</v>
       </c>
-      <c r="I141" s="3" t="n">
+      <c r="I141" s="2" t="n">
         <v>45720</v>
       </c>
       <c r="J141" t="inlineStr">
@@ -7956,7 +7956,7 @@
       <c r="H142" t="n">
         <v>72238369</v>
       </c>
-      <c r="I142" s="3" t="n">
+      <c r="I142" s="2" t="n">
         <v>45721</v>
       </c>
       <c r="J142" t="inlineStr">
@@ -8009,7 +8009,7 @@
       <c r="H143" t="n">
         <v>55623159</v>
       </c>
-      <c r="I143" s="3" t="n">
+      <c r="I143" s="2" t="n">
         <v>45722</v>
       </c>
       <c r="J143" t="inlineStr">
@@ -8062,7 +8062,7 @@
       <c r="H144" t="n">
         <v>106609976</v>
       </c>
-      <c r="I144" s="3" t="n">
+      <c r="I144" s="2" t="n">
         <v>45723</v>
       </c>
       <c r="J144" t="inlineStr">
@@ -8115,7 +8115,7 @@
       <c r="H145" t="n">
         <v>80803365</v>
       </c>
-      <c r="I145" s="3" t="n">
+      <c r="I145" s="2" t="n">
         <v>45726</v>
       </c>
       <c r="J145" t="inlineStr">
@@ -8168,7 +8168,7 @@
       <c r="H146" t="n">
         <v>58205458</v>
       </c>
-      <c r="I146" s="3" t="n">
+      <c r="I146" s="2" t="n">
         <v>45727</v>
       </c>
       <c r="J146" t="inlineStr">
@@ -8221,7 +8221,7 @@
       <c r="H147" t="n">
         <v>48134848</v>
       </c>
-      <c r="I147" s="3" t="n">
+      <c r="I147" s="2" t="n">
         <v>45728</v>
       </c>
       <c r="J147" t="inlineStr">
@@ -8274,7 +8274,7 @@
       <c r="H148" t="n">
         <v>43663314</v>
       </c>
-      <c r="I148" s="3" t="n">
+      <c r="I148" s="2" t="n">
         <v>45729</v>
       </c>
       <c r="J148" t="inlineStr">
@@ -8327,7 +8327,7 @@
       <c r="H149" t="n">
         <v>53881458</v>
       </c>
-      <c r="I149" s="3" t="n">
+      <c r="I149" s="2" t="n">
         <v>45733</v>
       </c>
       <c r="J149" t="inlineStr">
@@ -8380,7 +8380,7 @@
       <c r="H150" t="n">
         <v>42077765</v>
       </c>
-      <c r="I150" s="3" t="n">
+      <c r="I150" s="2" t="n">
         <v>45734</v>
       </c>
       <c r="J150" t="inlineStr">
@@ -8433,7 +8433,7 @@
       <c r="H151" t="n">
         <v>79292062</v>
       </c>
-      <c r="I151" s="3" t="n">
+      <c r="I151" s="2" t="n">
         <v>45735</v>
       </c>
       <c r="J151" t="inlineStr">
@@ -8486,7 +8486,7 @@
       <c r="H152" t="n">
         <v>51139907</v>
       </c>
-      <c r="I152" s="3" t="n">
+      <c r="I152" s="2" t="n">
         <v>45736</v>
       </c>
       <c r="J152" t="inlineStr">
@@ -8539,7 +8539,7 @@
       <c r="H153" t="n">
         <v>104561725</v>
       </c>
-      <c r="I153" s="3" t="n">
+      <c r="I153" s="2" t="n">
         <v>45737</v>
       </c>
       <c r="J153" t="inlineStr">
@@ -8592,7 +8592,7 @@
       <c r="H154" t="n">
         <v>57667042</v>
       </c>
-      <c r="I154" s="3" t="n">
+      <c r="I154" s="2" t="n">
         <v>45740</v>
       </c>
       <c r="J154" t="inlineStr">
@@ -8645,7 +8645,7 @@
       <c r="H155" t="n">
         <v>65862733</v>
       </c>
-      <c r="I155" s="3" t="n">
+      <c r="I155" s="2" t="n">
         <v>45741</v>
       </c>
       <c r="J155" t="inlineStr">
@@ -8698,7 +8698,7 @@
       <c r="H156" t="n">
         <v>51984215</v>
       </c>
-      <c r="I156" s="3" t="n">
+      <c r="I156" s="2" t="n">
         <v>45742</v>
       </c>
       <c r="J156" t="inlineStr">
@@ -8751,7 +8751,7 @@
       <c r="H157" t="n">
         <v>49392058</v>
       </c>
-      <c r="I157" s="3" t="n">
+      <c r="I157" s="2" t="n">
         <v>45743</v>
       </c>
       <c r="J157" t="inlineStr">
@@ -8804,7 +8804,7 @@
       <c r="H158" t="n">
         <v>43091944</v>
       </c>
-      <c r="I158" s="3" t="n">
+      <c r="I158" s="2" t="n">
         <v>45744</v>
       </c>
       <c r="J158" t="inlineStr">
@@ -8857,7 +8857,7 @@
       <c r="H159" t="n">
         <v>39979962</v>
       </c>
-      <c r="I159" s="3" t="n">
+      <c r="I159" s="2" t="n">
         <v>45748</v>
       </c>
       <c r="J159" t="inlineStr">
@@ -8910,7 +8910,7 @@
       <c r="H160" t="n">
         <v>49193068</v>
       </c>
-      <c r="I160" s="3" t="n">
+      <c r="I160" s="2" t="n">
         <v>45749</v>
       </c>
       <c r="J160" t="inlineStr">
@@ -8963,7 +8963,7 @@
       <c r="H161" t="n">
         <v>42640932</v>
       </c>
-      <c r="I161" s="3" t="n">
+      <c r="I161" s="2" t="n">
         <v>45750</v>
       </c>
       <c r="J161" t="inlineStr">
@@ -9016,7 +9016,7 @@
       <c r="H162" t="n">
         <v>51640942</v>
       </c>
-      <c r="I162" s="3" t="n">
+      <c r="I162" s="2" t="n">
         <v>45751</v>
       </c>
       <c r="J162" t="inlineStr">
@@ -9069,7 +9069,7 @@
       <c r="H163" t="n">
         <v>80391533</v>
       </c>
-      <c r="I163" s="3" t="n">
+      <c r="I163" s="2" t="n">
         <v>45754</v>
       </c>
       <c r="J163" t="inlineStr">
@@ -9122,7 +9122,7 @@
       <c r="H164" t="n">
         <v>40511090</v>
       </c>
-      <c r="I164" s="3" t="n">
+      <c r="I164" s="2" t="n">
         <v>45755</v>
       </c>
       <c r="J164" t="inlineStr">
@@ -9175,7 +9175,7 @@
       <c r="H165" t="n">
         <v>50595621</v>
       </c>
-      <c r="I165" s="3" t="n">
+      <c r="I165" s="2" t="n">
         <v>45756</v>
       </c>
       <c r="J165" t="inlineStr">
@@ -9228,7 +9228,7 @@
       <c r="H166" t="n">
         <v>48467923</v>
       </c>
-      <c r="I166" s="3" t="n">
+      <c r="I166" s="2" t="n">
         <v>45758</v>
       </c>
       <c r="J166" t="inlineStr">
@@ -9281,7 +9281,7 @@
       <c r="H167" t="n">
         <v>58278705</v>
       </c>
-      <c r="I167" s="3" t="n">
+      <c r="I167" s="2" t="n">
         <v>45762</v>
       </c>
       <c r="J167" t="inlineStr">
@@ -9334,7 +9334,7 @@
       <c r="H168" t="n">
         <v>34496997</v>
       </c>
-      <c r="I168" s="3" t="n">
+      <c r="I168" s="2" t="n">
         <v>45763</v>
       </c>
       <c r="J168" t="inlineStr">
@@ -9387,7 +9387,7 @@
       <c r="H169" t="n">
         <v>54100771</v>
       </c>
-      <c r="I169" s="3" t="n">
+      <c r="I169" s="2" t="n">
         <v>45764</v>
       </c>
       <c r="J169" t="inlineStr">
@@ -9440,7 +9440,7 @@
       <c r="H170" t="n">
         <v>169213523</v>
       </c>
-      <c r="I170" s="3" t="n">
+      <c r="I170" s="2" t="n">
         <v>45768</v>
       </c>
       <c r="J170" t="inlineStr">
@@ -9493,7 +9493,7 @@
       <c r="H171" t="n">
         <v>87624857</v>
       </c>
-      <c r="I171" s="3" t="n">
+      <c r="I171" s="2" t="n">
         <v>45769</v>
       </c>
       <c r="J171" t="inlineStr">
@@ -9546,7 +9546,7 @@
       <c r="H172" t="n">
         <v>97545142</v>
       </c>
-      <c r="I172" s="3" t="n">
+      <c r="I172" s="2" t="n">
         <v>45770</v>
       </c>
       <c r="J172" t="inlineStr">
@@ -9599,7 +9599,7 @@
       <c r="H173" t="n">
         <v>97071328</v>
       </c>
-      <c r="I173" s="3" t="n">
+      <c r="I173" s="2" t="n">
         <v>45771</v>
       </c>
       <c r="J173" t="inlineStr">
@@ -9652,7 +9652,7 @@
       <c r="H174" t="n">
         <v>103883639</v>
       </c>
-      <c r="I174" s="3" t="n">
+      <c r="I174" s="2" t="n">
         <v>45772</v>
       </c>
       <c r="J174" t="inlineStr">
@@ -9705,7 +9705,7 @@
       <c r="H175" t="n">
         <v>50214319</v>
       </c>
-      <c r="I175" s="3" t="n">
+      <c r="I175" s="2" t="n">
         <v>45775</v>
       </c>
       <c r="J175" t="inlineStr">
@@ -9758,7 +9758,7 @@
       <c r="H176" t="n">
         <v>51453372</v>
       </c>
-      <c r="I176" s="3" t="n">
+      <c r="I176" s="2" t="n">
         <v>45776</v>
       </c>
       <c r="J176" t="inlineStr">
@@ -9811,7 +9811,7 @@
       <c r="H177" t="n">
         <v>55292266</v>
       </c>
-      <c r="I177" s="3" t="n">
+      <c r="I177" s="2" t="n">
         <v>45777</v>
       </c>
       <c r="J177" t="inlineStr">
@@ -9864,7 +9864,7 @@
       <c r="H178" t="n">
         <v>41890615</v>
       </c>
-      <c r="I178" s="3" t="n">
+      <c r="I178" s="2" t="n">
         <v>45779</v>
       </c>
       <c r="J178" t="inlineStr">
@@ -9917,7 +9917,7 @@
       <c r="H179" t="n">
         <v>30069819</v>
       </c>
-      <c r="I179" s="3" t="n">
+      <c r="I179" s="2" t="n">
         <v>45782</v>
       </c>
       <c r="J179" t="inlineStr">
@@ -9970,7 +9970,7 @@
       <c r="H180" t="n">
         <v>59519033</v>
       </c>
-      <c r="I180" s="3" t="n">
+      <c r="I180" s="2" t="n">
         <v>45783</v>
       </c>
       <c r="J180" t="inlineStr">
@@ -10023,7 +10023,7 @@
       <c r="H181" t="n">
         <v>100130824</v>
       </c>
-      <c r="I181" s="3" t="n">
+      <c r="I181" s="2" t="n">
         <v>45784</v>
       </c>
       <c r="J181" t="inlineStr">
@@ -10076,7 +10076,7 @@
       <c r="H182" t="n">
         <v>64590237</v>
       </c>
-      <c r="I182" s="3" t="n">
+      <c r="I182" s="2" t="n">
         <v>45785</v>
       </c>
       <c r="J182" t="inlineStr">
@@ -10129,7 +10129,7 @@
       <c r="H183" t="n">
         <v>67885388</v>
       </c>
-      <c r="I183" s="3" t="n">
+      <c r="I183" s="2" t="n">
         <v>45786</v>
       </c>
       <c r="J183" t="inlineStr">
@@ -10182,7 +10182,7 @@
       <c r="H184" t="n">
         <v>88473615</v>
       </c>
-      <c r="I184" s="3" t="n">
+      <c r="I184" s="2" t="n">
         <v>45789</v>
       </c>
       <c r="J184" t="inlineStr">
@@ -10235,7 +10235,7 @@
       <c r="H185" t="n">
         <v>55125463</v>
       </c>
-      <c r="I185" s="3" t="n">
+      <c r="I185" s="2" t="n">
         <v>45790</v>
       </c>
       <c r="J185" t="inlineStr">
@@ -10288,7 +10288,7 @@
       <c r="H186" t="n">
         <v>97440289</v>
       </c>
-      <c r="I186" s="3" t="n">
+      <c r="I186" s="2" t="n">
         <v>45791</v>
       </c>
       <c r="J186" t="inlineStr">
@@ -10341,7 +10341,7 @@
       <c r="H187" t="n">
         <v>79233156</v>
       </c>
-      <c r="I187" s="3" t="n">
+      <c r="I187" s="2" t="n">
         <v>45792</v>
       </c>
       <c r="J187" t="inlineStr">
@@ -10394,7 +10394,7 @@
       <c r="H188" t="n">
         <v>77477145</v>
       </c>
-      <c r="I188" s="3" t="n">
+      <c r="I188" s="2" t="n">
         <v>45793</v>
       </c>
       <c r="J188" t="inlineStr">
@@ -10447,7 +10447,7 @@
       <c r="H189" t="n">
         <v>53000881</v>
       </c>
-      <c r="I189" s="3" t="n">
+      <c r="I189" s="2" t="n">
         <v>45796</v>
       </c>
       <c r="J189" t="inlineStr">
@@ -10500,7 +10500,7 @@
       <c r="H190" t="n">
         <v>64080954</v>
       </c>
-      <c r="I190" s="3" t="n">
+      <c r="I190" s="2" t="n">
         <v>45797</v>
       </c>
       <c r="J190" t="inlineStr">
@@ -10553,7 +10553,7 @@
       <c r="H191" t="n">
         <v>57465769</v>
       </c>
-      <c r="I191" s="3" t="n">
+      <c r="I191" s="2" t="n">
         <v>45798</v>
       </c>
       <c r="J191" t="inlineStr">
@@ -10606,7 +10606,7 @@
       <c r="H192" t="n">
         <v>43002318</v>
       </c>
-      <c r="I192" s="3" t="n">
+      <c r="I192" s="2" t="n">
         <v>45799</v>
       </c>
       <c r="J192" t="inlineStr">
@@ -10659,7 +10659,7 @@
       <c r="H193" t="n">
         <v>90422505</v>
       </c>
-      <c r="I193" s="3" t="n">
+      <c r="I193" s="2" t="n">
         <v>45800</v>
       </c>
       <c r="J193" t="inlineStr">
@@ -10712,7 +10712,7 @@
       <c r="H194" t="n">
         <v>126038462</v>
       </c>
-      <c r="I194" s="3" t="n">
+      <c r="I194" s="2" t="n">
         <v>45803</v>
       </c>
       <c r="J194" t="inlineStr">
@@ -10765,7 +10765,7 @@
       <c r="H195" t="n">
         <v>124896028</v>
       </c>
-      <c r="I195" s="3" t="n">
+      <c r="I195" s="2" t="n">
         <v>45804</v>
       </c>
       <c r="J195" t="inlineStr">
@@ -10818,7 +10818,7 @@
       <c r="H196" t="n">
         <v>161911717</v>
       </c>
-      <c r="I196" s="3" t="n">
+      <c r="I196" s="2" t="n">
         <v>45805</v>
       </c>
       <c r="J196" t="inlineStr">
@@ -10871,7 +10871,7 @@
       <c r="H197" t="n">
         <v>105011188</v>
       </c>
-      <c r="I197" s="3" t="n">
+      <c r="I197" s="2" t="n">
         <v>45806</v>
       </c>
       <c r="J197" t="inlineStr">
@@ -10924,7 +10924,7 @@
       <c r="H198" t="n">
         <v>536489431</v>
       </c>
-      <c r="I198" s="3" t="n">
+      <c r="I198" s="2" t="n">
         <v>45807</v>
       </c>
       <c r="J198" t="inlineStr">
@@ -10977,7 +10977,7 @@
       <c r="H199" t="n">
         <v>171657905</v>
       </c>
-      <c r="I199" s="3" t="n">
+      <c r="I199" s="2" t="n">
         <v>45810</v>
       </c>
       <c r="J199" t="inlineStr">
@@ -11030,7 +11030,7 @@
       <c r="H200" t="n">
         <v>165730448</v>
       </c>
-      <c r="I200" s="3" t="n">
+      <c r="I200" s="2" t="n">
         <v>45811</v>
       </c>
       <c r="J200" t="inlineStr">
@@ -11083,7 +11083,7 @@
       <c r="H201" t="n">
         <v>125224353</v>
       </c>
-      <c r="I201" s="3" t="n">
+      <c r="I201" s="2" t="n">
         <v>45812</v>
       </c>
       <c r="J201" t="inlineStr">
@@ -11136,7 +11136,7 @@
       <c r="H202" t="n">
         <v>116057135</v>
       </c>
-      <c r="I202" s="3" t="n">
+      <c r="I202" s="2" t="n">
         <v>45813</v>
       </c>
       <c r="J202" t="inlineStr">
@@ -11189,7 +11189,7 @@
       <c r="H203" t="n">
         <v>75348107</v>
       </c>
-      <c r="I203" s="3" t="n">
+      <c r="I203" s="2" t="n">
         <v>45814</v>
       </c>
       <c r="J203" t="inlineStr">
@@ -11242,7 +11242,7 @@
       <c r="H204" t="n">
         <v>107525192</v>
       </c>
-      <c r="I204" s="3" t="n">
+      <c r="I204" s="2" t="n">
         <v>45817</v>
       </c>
       <c r="J204" t="inlineStr">
@@ -11295,7 +11295,7 @@
       <c r="H205" t="n">
         <v>157049300</v>
       </c>
-      <c r="I205" s="3" t="n">
+      <c r="I205" s="2" t="n">
         <v>45818</v>
       </c>
       <c r="J205" t="inlineStr">
@@ -11348,7 +11348,7 @@
       <c r="H206" t="n">
         <v>99297135</v>
       </c>
-      <c r="I206" s="3" t="n">
+      <c r="I206" s="2" t="n">
         <v>45819</v>
       </c>
       <c r="J206" t="inlineStr">
@@ -11401,7 +11401,7 @@
       <c r="H207" t="n">
         <v>90785452</v>
       </c>
-      <c r="I207" s="3" t="n">
+      <c r="I207" s="2" t="n">
         <v>45820</v>
       </c>
       <c r="J207" t="inlineStr">
@@ -11454,7 +11454,7 @@
       <c r="H208" t="n">
         <v>89307151</v>
       </c>
-      <c r="I208" s="3" t="n">
+      <c r="I208" s="2" t="n">
         <v>45821</v>
       </c>
       <c r="J208" t="inlineStr">
@@ -11507,7 +11507,7 @@
       <c r="H209" t="n">
         <v>82312525</v>
       </c>
-      <c r="I209" s="3" t="n">
+      <c r="I209" s="2" t="n">
         <v>45824</v>
       </c>
       <c r="J209" t="inlineStr">
@@ -11560,7 +11560,7 @@
       <c r="H210" t="n">
         <v>62032127</v>
       </c>
-      <c r="I210" s="3" t="n">
+      <c r="I210" s="2" t="n">
         <v>45825</v>
       </c>
       <c r="J210" t="inlineStr">
@@ -11613,7 +11613,7 @@
       <c r="H211" t="n">
         <v>49079799</v>
       </c>
-      <c r="I211" s="3" t="n">
+      <c r="I211" s="2" t="n">
         <v>45826</v>
       </c>
       <c r="J211" t="inlineStr">
@@ -11666,7 +11666,7 @@
       <c r="H212" t="n">
         <v>90457856</v>
       </c>
-      <c r="I212" s="3" t="n">
+      <c r="I212" s="2" t="n">
         <v>45827</v>
       </c>
       <c r="J212" t="inlineStr">
@@ -11719,7 +11719,7 @@
       <c r="H213" t="n">
         <v>155042048</v>
       </c>
-      <c r="I213" s="3" t="n">
+      <c r="I213" s="2" t="n">
         <v>45828</v>
       </c>
       <c r="J213" t="inlineStr">
@@ -11772,7 +11772,7 @@
       <c r="H214" t="n">
         <v>47462713</v>
       </c>
-      <c r="I214" s="3" t="n">
+      <c r="I214" s="2" t="n">
         <v>45831</v>
       </c>
       <c r="J214" t="inlineStr">
@@ -11825,7 +11825,7 @@
       <c r="H215" t="n">
         <v>83742518</v>
       </c>
-      <c r="I215" s="3" t="n">
+      <c r="I215" s="2" t="n">
         <v>45832</v>
       </c>
       <c r="J215" t="inlineStr">
@@ -11878,7 +11878,7 @@
       <c r="H216" t="n">
         <v>51167086</v>
       </c>
-      <c r="I216" s="3" t="n">
+      <c r="I216" s="2" t="n">
         <v>45833</v>
       </c>
       <c r="J216" t="inlineStr">
@@ -11931,7 +11931,7 @@
       <c r="H217" t="n">
         <v>63446312</v>
       </c>
-      <c r="I217" s="3" t="n">
+      <c r="I217" s="2" t="n">
         <v>45834</v>
       </c>
       <c r="J217" t="inlineStr">
@@ -11984,7 +11984,7 @@
       <c r="H218" t="n">
         <v>157053714</v>
       </c>
-      <c r="I218" s="3" t="n">
+      <c r="I218" s="2" t="n">
         <v>45835</v>
       </c>
       <c r="J218" t="inlineStr">
@@ -12037,7 +12037,7 @@
       <c r="H219" t="n">
         <v>99308749</v>
       </c>
-      <c r="I219" s="3" t="n">
+      <c r="I219" s="2" t="n">
         <v>45838</v>
       </c>
       <c r="J219" t="inlineStr">
@@ -12090,7 +12090,7 @@
       <c r="H220" t="n">
         <v>48940171</v>
       </c>
-      <c r="I220" s="3" t="n">
+      <c r="I220" s="2" t="n">
         <v>45839</v>
       </c>
       <c r="J220" t="inlineStr">
@@ -12143,7 +12143,7 @@
       <c r="H221" t="n">
         <v>72627565</v>
       </c>
-      <c r="I221" s="3" t="n">
+      <c r="I221" s="2" t="n">
         <v>45840</v>
       </c>
       <c r="J221" t="inlineStr">
@@ -12196,7 +12196,7 @@
       <c r="H222" t="n">
         <v>47789302</v>
       </c>
-      <c r="I222" s="3" t="n">
+      <c r="I222" s="2" t="n">
         <v>45841</v>
       </c>
       <c r="J222" t="inlineStr">
@@ -12249,7 +12249,7 @@
       <c r="H223" t="n">
         <v>32039017</v>
       </c>
-      <c r="I223" s="3" t="n">
+      <c r="I223" s="2" t="n">
         <v>45842</v>
       </c>
       <c r="J223" t="inlineStr">
@@ -12302,7 +12302,7 @@
       <c r="H224" t="n">
         <v>41571440</v>
       </c>
-      <c r="I224" s="3" t="n">
+      <c r="I224" s="2" t="n">
         <v>45845</v>
       </c>
       <c r="J224" t="inlineStr">
@@ -12355,7 +12355,7 @@
       <c r="H225" t="n">
         <v>40556159</v>
       </c>
-      <c r="I225" s="3" t="n">
+      <c r="I225" s="2" t="n">
         <v>45846</v>
       </c>
       <c r="J225" t="inlineStr">
@@ -12408,7 +12408,7 @@
       <c r="H226" t="n">
         <v>39705171</v>
       </c>
-      <c r="I226" s="3" t="n">
+      <c r="I226" s="2" t="n">
         <v>45847</v>
       </c>
       <c r="J226" t="inlineStr">
@@ -12461,7 +12461,7 @@
       <c r="H227" t="n">
         <v>30808538</v>
       </c>
-      <c r="I227" s="3" t="n">
+      <c r="I227" s="2" t="n">
         <v>45848</v>
       </c>
       <c r="J227" t="inlineStr">
@@ -12514,7 +12514,7 @@
       <c r="H228" t="n">
         <v>32604930</v>
       </c>
-      <c r="I228" s="3" t="n">
+      <c r="I228" s="2" t="n">
         <v>45849</v>
       </c>
       <c r="J228" t="inlineStr">
@@ -12567,7 +12567,7 @@
       <c r="H229" t="n">
         <v>37670805</v>
       </c>
-      <c r="I229" s="3" t="n">
+      <c r="I229" s="2" t="n">
         <v>45852</v>
       </c>
       <c r="J229" t="inlineStr">
@@ -12620,7 +12620,7 @@
       <c r="H230" t="n">
         <v>67875212</v>
       </c>
-      <c r="I230" s="3" t="n">
+      <c r="I230" s="2" t="n">
         <v>45853</v>
       </c>
       <c r="J230" t="inlineStr">
@@ -12673,7 +12673,7 @@
       <c r="H231" t="n">
         <v>52277504</v>
       </c>
-      <c r="I231" s="3" t="n">
+      <c r="I231" s="2" t="n">
         <v>45854</v>
       </c>
       <c r="J231" t="inlineStr">
@@ -12726,7 +12726,7 @@
       <c r="H232" t="n">
         <v>31253597</v>
       </c>
-      <c r="I232" s="3" t="n">
+      <c r="I232" s="2" t="n">
         <v>45855</v>
       </c>
       <c r="J232" t="inlineStr">
@@ -12779,7 +12779,7 @@
       <c r="H233" t="n">
         <v>36973591</v>
       </c>
-      <c r="I233" s="3" t="n">
+      <c r="I233" s="2" t="n">
         <v>45856</v>
       </c>
       <c r="J233" t="inlineStr">
@@ -12832,7 +12832,7 @@
       <c r="H234" t="n">
         <v>35567782</v>
       </c>
-      <c r="I234" s="3" t="n">
+      <c r="I234" s="2" t="n">
         <v>45859</v>
       </c>
       <c r="J234" t="inlineStr">
@@ -12885,7 +12885,7 @@
       <c r="H235" t="n">
         <v>35572825</v>
       </c>
-      <c r="I235" s="3" t="n">
+      <c r="I235" s="2" t="n">
         <v>45860</v>
       </c>
       <c r="J235" t="inlineStr">
@@ -12938,7 +12938,7 @@
       <c r="H236" t="n">
         <v>32547549</v>
       </c>
-      <c r="I236" s="3" t="n">
+      <c r="I236" s="2" t="n">
         <v>45861</v>
       </c>
       <c r="J236" t="inlineStr">
@@ -12991,7 +12991,7 @@
       <c r="H237" t="n">
         <v>25716467</v>
       </c>
-      <c r="I237" s="3" t="n">
+      <c r="I237" s="2" t="n">
         <v>45862</v>
       </c>
       <c r="J237" t="inlineStr">
@@ -13044,7 +13044,7 @@
       <c r="H238" t="n">
         <v>54993410</v>
       </c>
-      <c r="I238" s="3" t="n">
+      <c r="I238" s="2" t="n">
         <v>45863</v>
       </c>
       <c r="J238" t="inlineStr">
@@ -13097,7 +13097,7 @@
       <c r="H239" t="n">
         <v>63653757</v>
       </c>
-      <c r="I239" s="3" t="n">
+      <c r="I239" s="2" t="n">
         <v>45866</v>
       </c>
       <c r="J239" t="inlineStr">
@@ -13150,7 +13150,7 @@
       <c r="H240" t="n">
         <v>53119837</v>
       </c>
-      <c r="I240" s="3" t="n">
+      <c r="I240" s="2" t="n">
         <v>45867</v>
       </c>
       <c r="J240" t="inlineStr">
@@ -13203,7 +13203,7 @@
       <c r="H241" t="n">
         <v>26017961</v>
       </c>
-      <c r="I241" s="3" t="n">
+      <c r="I241" s="2" t="n">
         <v>45868</v>
       </c>
       <c r="J241" t="inlineStr">
@@ -13256,7 +13256,7 @@
       <c r="H242" t="n">
         <v>51864787</v>
       </c>
-      <c r="I242" s="3" t="n">
+      <c r="I242" s="2" t="n">
         <v>45869</v>
       </c>
       <c r="J242" t="inlineStr">
@@ -13309,7 +13309,7 @@
       <c r="H243" t="n">
         <v>282277682</v>
       </c>
-      <c r="I243" s="3" t="n">
+      <c r="I243" s="2" t="n">
         <v>45870</v>
       </c>
       <c r="J243" t="inlineStr">
@@ -13362,7 +13362,7 @@
       <c r="H244" t="n">
         <v>71314001</v>
       </c>
-      <c r="I244" s="3" t="n">
+      <c r="I244" s="2" t="n">
         <v>45873</v>
       </c>
       <c r="J244" t="inlineStr">
@@ -13415,7 +13415,7 @@
       <c r="H245" t="n">
         <v>49067811</v>
       </c>
-      <c r="I245" s="3" t="n">
+      <c r="I245" s="2" t="n">
         <v>45874</v>
       </c>
       <c r="J245" t="inlineStr">
@@ -13468,7 +13468,7 @@
       <c r="H246" t="n">
         <v>47015454</v>
       </c>
-      <c r="I246" s="3" t="n">
+      <c r="I246" s="2" t="n">
         <v>45875</v>
       </c>
       <c r="J246" t="inlineStr">
@@ -13521,7 +13521,7 @@
       <c r="H247" t="n">
         <v>75356463</v>
       </c>
-      <c r="I247" s="3" t="n">
+      <c r="I247" s="2" t="n">
         <v>45876</v>
       </c>
       <c r="J247" t="inlineStr">
@@ -13574,7 +13574,7 @@
       <c r="H248" t="n">
         <v>44197301</v>
       </c>
-      <c r="I248" s="3" t="n">
+      <c r="I248" s="2" t="n">
         <v>45877</v>
       </c>
       <c r="J248" t="inlineStr">
@@ -13627,7 +13627,7 @@
       <c r="H249" t="n">
         <v>56151812</v>
       </c>
-      <c r="I249" s="3" t="n">
+      <c r="I249" s="2" t="n">
         <v>45880</v>
       </c>
       <c r="J249" t="inlineStr">
@@ -13680,7 +13680,7 @@
       <c r="H250" t="n">
         <v>97524524</v>
       </c>
-      <c r="I250" s="3" t="n">
+      <c r="I250" s="2" t="n">
         <v>45881</v>
       </c>
       <c r="J250" t="inlineStr">
@@ -13733,7 +13733,7 @@
       <c r="H251" t="n">
         <v>171463838</v>
       </c>
-      <c r="I251" s="3" t="n">
+      <c r="I251" s="2" t="n">
         <v>45882</v>
       </c>
       <c r="J251" t="inlineStr">
@@ -13786,7 +13786,7 @@
       <c r="H252" t="n">
         <v>61040027</v>
       </c>
-      <c r="I252" s="3" t="n">
+      <c r="I252" s="2" t="n">
         <v>45883</v>
       </c>
       <c r="J252" t="inlineStr">
@@ -13839,7 +13839,7 @@
       <c r="H253" t="n">
         <v>174705889</v>
       </c>
-      <c r="I253" s="3" t="n">
+      <c r="I253" s="2" t="n">
         <v>45887</v>
       </c>
       <c r="J253" t="inlineStr">
@@ -13892,7 +13892,7 @@
       <c r="H254" t="n">
         <v>100028906</v>
       </c>
-      <c r="I254" s="3" t="n">
+      <c r="I254" s="2" t="n">
         <v>45888</v>
       </c>
       <c r="J254" t="inlineStr">
@@ -13945,7 +13945,7 @@
       <c r="H255" t="n">
         <v>58658385</v>
       </c>
-      <c r="I255" s="3" t="n">
+      <c r="I255" s="2" t="n">
         <v>45889</v>
       </c>
       <c r="J255" t="inlineStr">
@@ -13998,7 +13998,7 @@
       <c r="H256" t="n">
         <v>52767620</v>
       </c>
-      <c r="I256" s="3" t="n">
+      <c r="I256" s="2" t="n">
         <v>45890</v>
       </c>
       <c r="J256" t="inlineStr">
@@ -14051,7 +14051,7 @@
       <c r="H257" t="n">
         <v>67221130</v>
       </c>
-      <c r="I257" s="3" t="n">
+      <c r="I257" s="2" t="n">
         <v>45891</v>
       </c>
       <c r="J257" t="inlineStr">
@@ -14104,7 +14104,7 @@
       <c r="H258" t="n">
         <v>54657124</v>
       </c>
-      <c r="I258" s="3" t="n">
+      <c r="I258" s="2" t="n">
         <v>45894</v>
       </c>
       <c r="J258" t="inlineStr">
@@ -14157,7 +14157,7 @@
       <c r="H259" t="n">
         <v>53829442</v>
       </c>
-      <c r="I259" s="3" t="n">
+      <c r="I259" s="2" t="n">
         <v>45895</v>
       </c>
       <c r="J259" t="inlineStr">
@@ -14210,7 +14210,7 @@
       <c r="H260" t="n">
         <v>57413447</v>
       </c>
-      <c r="I260" s="3" t="n">
+      <c r="I260" s="2" t="n">
         <v>45897</v>
       </c>
       <c r="J260" t="inlineStr">
@@ -14263,7 +14263,7 @@
       <c r="H261" t="n">
         <v>65867650</v>
       </c>
-      <c r="I261" s="3" t="n">
+      <c r="I261" s="2" t="n">
         <v>45898</v>
       </c>
       <c r="J261" t="inlineStr">
@@ -14316,7 +14316,7 @@
       <c r="H262" t="n">
         <v>62476377</v>
       </c>
-      <c r="I262" s="3" t="n">
+      <c r="I262" s="2" t="n">
         <v>45901</v>
       </c>
       <c r="J262" t="inlineStr">
@@ -14369,7 +14369,7 @@
       <c r="H263" t="n">
         <v>72436469</v>
       </c>
-      <c r="I263" s="3" t="n">
+      <c r="I263" s="2" t="n">
         <v>45902</v>
       </c>
       <c r="J263" t="inlineStr">
@@ -14422,7 +14422,7 @@
       <c r="H264" t="n">
         <v>43830688</v>
       </c>
-      <c r="I264" s="3" t="n">
+      <c r="I264" s="2" t="n">
         <v>45903</v>
       </c>
       <c r="J264" t="inlineStr">
@@ -14475,7 +14475,7 @@
       <c r="H265" t="n">
         <v>45224146</v>
       </c>
-      <c r="I265" s="3" t="n">
+      <c r="I265" s="2" t="n">
         <v>45904</v>
       </c>
       <c r="J265" t="inlineStr">
@@ -14528,7 +14528,7 @@
       <c r="H266" t="n">
         <v>36826585</v>
       </c>
-      <c r="I266" s="3" t="n">
+      <c r="I266" s="2" t="n">
         <v>45905</v>
       </c>
       <c r="J266" t="inlineStr">
@@ -14581,7 +14581,7 @@
       <c r="H267" t="n">
         <v>31064465</v>
       </c>
-      <c r="I267" s="3" t="n">
+      <c r="I267" s="2" t="n">
         <v>45908</v>
       </c>
       <c r="J267" t="inlineStr">
@@ -14634,7 +14634,7 @@
       <c r="H268" t="n">
         <v>28259628</v>
       </c>
-      <c r="I268" s="3" t="n">
+      <c r="I268" s="2" t="n">
         <v>45909</v>
       </c>
       <c r="J268" t="inlineStr">
@@ -14687,7 +14687,7 @@
       <c r="H269" t="n">
         <v>36829592</v>
       </c>
-      <c r="I269" s="3" t="n">
+      <c r="I269" s="2" t="n">
         <v>45910</v>
       </c>
       <c r="J269" t="inlineStr">
@@ -14740,7 +14740,7 @@
       <c r="H270" t="n">
         <v>35511499</v>
       </c>
-      <c r="I270" s="3" t="n">
+      <c r="I270" s="2" t="n">
         <v>45911</v>
       </c>
       <c r="J270" t="inlineStr">
@@ -14793,7 +14793,7 @@
       <c r="H271" t="n">
         <v>30646622</v>
       </c>
-      <c r="I271" s="3" t="n">
+      <c r="I271" s="2" t="n">
         <v>45912</v>
       </c>
       <c r="J271" t="inlineStr">
@@ -14846,7 +14846,7 @@
       <c r="H272" t="n">
         <v>47583621</v>
       </c>
-      <c r="I272" s="3" t="n">
+      <c r="I272" s="2" t="n">
         <v>45915</v>
       </c>
       <c r="J272" t="inlineStr">
@@ -14899,7 +14899,7 @@
       <c r="H273" t="n">
         <v>83823836</v>
       </c>
-      <c r="I273" s="3" t="n">
+      <c r="I273" s="2" t="n">
         <v>45916</v>
       </c>
       <c r="J273" t="inlineStr">
@@ -14952,7 +14952,7 @@
       <c r="H274" t="n">
         <v>62170240</v>
       </c>
-      <c r="I274" s="3" t="n">
+      <c r="I274" s="2" t="n">
         <v>45917</v>
       </c>
       <c r="J274" t="inlineStr">
@@ -15005,7 +15005,7 @@
       <c r="H275" t="n">
         <v>34201666</v>
       </c>
-      <c r="I275" s="3" t="n">
+      <c r="I275" s="2" t="n">
         <v>45918</v>
       </c>
       <c r="J275" t="inlineStr">
@@ -15058,7 +15058,7 @@
       <c r="H276" t="n">
         <v>84296198</v>
       </c>
-      <c r="I276" s="3" t="n">
+      <c r="I276" s="2" t="n">
         <v>45919</v>
       </c>
       <c r="J276" t="inlineStr">
@@ -15111,7 +15111,7 @@
       <c r="H277" t="n">
         <v>61536801</v>
       </c>
-      <c r="I277" s="3" t="n">
+      <c r="I277" s="2" t="n">
         <v>45922</v>
       </c>
       <c r="J277" t="inlineStr">
@@ -15164,7 +15164,7 @@
       <c r="H278" t="n">
         <v>42951519</v>
       </c>
-      <c r="I278" s="3" t="n">
+      <c r="I278" s="2" t="n">
         <v>45923</v>
       </c>
       <c r="J278" t="inlineStr">
@@ -15217,7 +15217,7 @@
       <c r="H279" t="n">
         <v>36713845</v>
       </c>
-      <c r="I279" s="3" t="n">
+      <c r="I279" s="2" t="n">
         <v>45924</v>
       </c>
       <c r="J279" t="inlineStr">
@@ -15270,7 +15270,7 @@
       <c r="H280" t="n">
         <v>38004835</v>
       </c>
-      <c r="I280" s="3" t="n">
+      <c r="I280" s="2" t="n">
         <v>45925</v>
       </c>
       <c r="J280" t="inlineStr">
@@ -15323,7 +15323,7 @@
       <c r="H281" t="n">
         <v>54141564</v>
       </c>
-      <c r="I281" s="3" t="n">
+      <c r="I281" s="2" t="n">
         <v>45926</v>
       </c>
       <c r="J281" t="inlineStr">
@@ -15376,7 +15376,7 @@
       <c r="H282" t="n">
         <v>49278897</v>
       </c>
-      <c r="I282" s="3" t="n">
+      <c r="I282" s="2" t="n">
         <v>45929</v>
       </c>
       <c r="J282" t="inlineStr">
@@ -15429,7 +15429,7 @@
       <c r="H283" t="n">
         <v>57370118</v>
       </c>
-      <c r="I283" s="3" t="n">
+      <c r="I283" s="2" t="n">
         <v>45930</v>
       </c>
       <c r="J283" t="inlineStr">
@@ -15482,7 +15482,7 @@
       <c r="H284" t="n">
         <v>45989378</v>
       </c>
-      <c r="I284" s="3" t="n">
+      <c r="I284" s="2" t="n">
         <v>45931</v>
       </c>
       <c r="J284" t="inlineStr">
@@ -15535,7 +15535,7 @@
       <c r="H285" t="n">
         <v>68751486</v>
       </c>
-      <c r="I285" s="3" t="n">
+      <c r="I285" s="2" t="n">
         <v>45933</v>
       </c>
       <c r="J285" t="inlineStr">
@@ -15588,7 +15588,7 @@
       <c r="H286" t="n">
         <v>44695672</v>
       </c>
-      <c r="I286" s="3" t="n">
+      <c r="I286" s="2" t="n">
         <v>45936</v>
       </c>
       <c r="J286" t="inlineStr">
@@ -15641,7 +15641,7 @@
       <c r="H287" t="n">
         <v>50380035</v>
       </c>
-      <c r="I287" s="3" t="n">
+      <c r="I287" s="2" t="n">
         <v>45937</v>
       </c>
       <c r="J287" t="inlineStr">
@@ -15694,7 +15694,7 @@
       <c r="H288" t="n">
         <v>60256029</v>
       </c>
-      <c r="I288" s="3" t="n">
+      <c r="I288" s="2" t="n">
         <v>45938</v>
       </c>
       <c r="J288" t="inlineStr">
@@ -15747,7 +15747,7 @@
       <c r="H289" t="n">
         <v>63378104</v>
       </c>
-      <c r="I289" s="3" t="n">
+      <c r="I289" s="2" t="n">
         <v>45939</v>
       </c>
       <c r="J289" t="inlineStr">
@@ -15800,7 +15800,7 @@
       <c r="H290" t="n">
         <v>58774401</v>
       </c>
-      <c r="I290" s="3" t="n">
+      <c r="I290" s="2" t="n">
         <v>45940</v>
       </c>
       <c r="J290" t="inlineStr">
@@ -15853,7 +15853,7 @@
       <c r="H291" t="n">
         <v>43991850</v>
       </c>
-      <c r="I291" s="3" t="n">
+      <c r="I291" s="2" t="n">
         <v>45943</v>
       </c>
       <c r="J291" t="inlineStr">
@@ -15906,7 +15906,7 @@
       <c r="H292" t="n">
         <v>40526897</v>
       </c>
-      <c r="I292" s="3" t="n">
+      <c r="I292" s="2" t="n">
         <v>45944</v>
       </c>
       <c r="J292" t="inlineStr">
@@ -15959,7 +15959,7 @@
       <c r="H293" t="n">
         <v>56429168</v>
       </c>
-      <c r="I293" s="3" t="n">
+      <c r="I293" s="2" t="n">
         <v>45945</v>
       </c>
       <c r="J293" t="inlineStr">
@@ -16012,7 +16012,7 @@
       <c r="H294" t="n">
         <v>48716419</v>
       </c>
-      <c r="I294" s="3" t="n">
+      <c r="I294" s="2" t="n">
         <v>45946</v>
       </c>
       <c r="J294" t="inlineStr">
@@ -16065,7 +16065,7 @@
       <c r="H295" t="n">
         <v>173497742</v>
       </c>
-      <c r="I295" s="3" t="n">
+      <c r="I295" s="2" t="n">
         <v>45947</v>
       </c>
       <c r="J295" t="inlineStr">
@@ -16118,7 +16118,7 @@
       <c r="H296" t="n">
         <v>34157489</v>
       </c>
-      <c r="I296" s="3" t="n">
+      <c r="I296" s="2" t="n">
         <v>45950</v>
       </c>
       <c r="J296" t="inlineStr">
@@ -16171,7 +16171,7 @@
       <c r="H297" t="n">
         <v>22587338</v>
       </c>
-      <c r="I297" s="3" t="n">
+      <c r="I297" s="2" t="n">
         <v>45951</v>
       </c>
       <c r="J297" t="inlineStr">
@@ -16224,7 +16224,7 @@
       <c r="H298" t="n">
         <v>75705464</v>
       </c>
-      <c r="I298" s="3" t="n">
+      <c r="I298" s="2" t="n">
         <v>45953</v>
       </c>
       <c r="J298" t="inlineStr">
@@ -16277,7 +16277,7 @@
       <c r="H299" t="n">
         <v>44166882</v>
       </c>
-      <c r="I299" s="3" t="n">
+      <c r="I299" s="2" t="n">
         <v>45954</v>
       </c>
       <c r="J299" t="inlineStr">
@@ -16330,7 +16330,7 @@
       <c r="H300" t="n">
         <v>24502140</v>
       </c>
-      <c r="I300" s="3" t="n">
+      <c r="I300" s="2" t="n">
         <v>45957</v>
       </c>
       <c r="J300" t="inlineStr">
@@ -16383,7 +16383,7 @@
       <c r="H301" t="n">
         <v>134110189</v>
       </c>
-      <c r="I301" s="3" t="n">
+      <c r="I301" s="2" t="n">
         <v>45958</v>
       </c>
       <c r="J301" t="inlineStr">
@@ -16436,7 +16436,7 @@
       <c r="H302" t="n">
         <v>154556298</v>
       </c>
-      <c r="I302" s="3" t="n">
+      <c r="I302" s="2" t="n">
         <v>45959</v>
       </c>
       <c r="J302" t="inlineStr">
@@ -16489,7 +16489,7 @@
       <c r="H303" t="n">
         <v>82432227</v>
       </c>
-      <c r="I303" s="3" t="n">
+      <c r="I303" s="2" t="n">
         <v>45960</v>
       </c>
       <c r="J303" t="inlineStr">
@@ -16542,7 +16542,7 @@
       <c r="H304" t="n">
         <v>107495287</v>
       </c>
-      <c r="I304" s="3" t="n">
+      <c r="I304" s="2" t="n">
         <v>45961</v>
       </c>
       <c r="J304" t="inlineStr">
@@ -16595,7 +16595,7 @@
       <c r="H305" t="n">
         <v>74454953</v>
       </c>
-      <c r="I305" s="3" t="n">
+      <c r="I305" s="2" t="n">
         <v>45964</v>
       </c>
       <c r="J305" t="inlineStr">
@@ -16648,7 +16648,7 @@
       <c r="H306" t="n">
         <v>316562869</v>
       </c>
-      <c r="I306" s="3" t="n">
+      <c r="I306" s="2" t="n">
         <v>45965</v>
       </c>
       <c r="J306" t="inlineStr">
@@ -16701,7 +16701,7 @@
       <c r="H307" t="n">
         <v>144210187</v>
       </c>
-      <c r="I307" s="3" t="n">
+      <c r="I307" s="2" t="n">
         <v>45967</v>
       </c>
       <c r="J307" t="inlineStr">
@@ -16754,7 +16754,7 @@
       <c r="H308" t="n">
         <v>122445076</v>
       </c>
-      <c r="I308" s="3" t="n">
+      <c r="I308" s="2" t="n">
         <v>45968</v>
       </c>
       <c r="J308" t="inlineStr">
@@ -16807,7 +16807,7 @@
       <c r="H309" t="n">
         <v>62625975</v>
       </c>
-      <c r="I309" s="3" t="n">
+      <c r="I309" s="2" t="n">
         <v>45971</v>
       </c>
       <c r="J309" t="inlineStr">
@@ -16860,7 +16860,7 @@
       <c r="H310" t="n">
         <v>50200645</v>
       </c>
-      <c r="I310" s="3" t="n">
+      <c r="I310" s="2" t="n">
         <v>45972</v>
       </c>
       <c r="J310" t="inlineStr">
@@ -16913,7 +16913,7 @@
       <c r="H311" t="n">
         <v>52722883</v>
       </c>
-      <c r="I311" s="3" t="n">
+      <c r="I311" s="2" t="n">
         <v>45973</v>
       </c>
       <c r="J311" t="inlineStr">
@@ -16966,7 +16966,7 @@
       <c r="H312" t="n">
         <v>40023986</v>
       </c>
-      <c r="I312" s="3" t="n">
+      <c r="I312" s="2" t="n">
         <v>45974</v>
       </c>
       <c r="J312" t="inlineStr">
@@ -17019,7 +17019,7 @@
       <c r="H313" t="n">
         <v>40924386</v>
       </c>
-      <c r="I313" s="3" t="n">
+      <c r="I313" s="2" t="n">
         <v>45975</v>
       </c>
       <c r="J313" t="inlineStr">
@@ -17072,7 +17072,7 @@
       <c r="H314" t="n">
         <v>35830648</v>
       </c>
-      <c r="I314" s="3" t="n">
+      <c r="I314" s="2" t="n">
         <v>45978</v>
       </c>
       <c r="J314" t="inlineStr">
@@ -17125,7 +17125,7 @@
       <c r="H315" t="n">
         <v>29428363</v>
       </c>
-      <c r="I315" s="3" t="n">
+      <c r="I315" s="2" t="n">
         <v>45979</v>
       </c>
       <c r="J315" t="inlineStr">
@@ -17178,7 +17178,7 @@
       <c r="H316" t="n">
         <v>35700982</v>
       </c>
-      <c r="I316" s="3" t="n">
+      <c r="I316" s="2" t="n">
         <v>45980</v>
       </c>
       <c r="J316" t="inlineStr">
@@ -17231,7 +17231,7 @@
       <c r="H317" t="n">
         <v>37412490</v>
       </c>
-      <c r="I317" s="3" t="n">
+      <c r="I317" s="2" t="n">
         <v>45981</v>
       </c>
       <c r="J317" t="inlineStr">
@@ -17284,7 +17284,7 @@
       <c r="H318" t="n">
         <v>42719729</v>
       </c>
-      <c r="I318" s="3" t="n">
+      <c r="I318" s="2" t="n">
         <v>45982</v>
       </c>
       <c r="J318" t="inlineStr">
@@ -17337,7 +17337,7 @@
       <c r="H319" t="n">
         <v>95958383</v>
       </c>
-      <c r="I319" s="3" t="n">
+      <c r="I319" s="2" t="n">
         <v>45985</v>
       </c>
       <c r="J319" t="inlineStr">
@@ -17390,7 +17390,7 @@
       <c r="H320" t="n">
         <v>36428307</v>
       </c>
-      <c r="I320" s="3" t="n">
+      <c r="I320" s="2" t="n">
         <v>45986</v>
       </c>
       <c r="J320" t="inlineStr">
@@ -17443,7 +17443,7 @@
       <c r="H321" t="n">
         <v>43639834</v>
       </c>
-      <c r="I321" s="3" t="n">
+      <c r="I321" s="2" t="n">
         <v>45987</v>
       </c>
       <c r="J321" t="inlineStr">
@@ -17496,7 +17496,7 @@
       <c r="H322" t="n">
         <v>28492915</v>
       </c>
-      <c r="I322" s="3" t="n">
+      <c r="I322" s="2" t="n">
         <v>45988</v>
       </c>
       <c r="J322" t="inlineStr">
@@ -17549,7 +17549,7 @@
       <c r="H323" t="n">
         <v>52380481</v>
       </c>
-      <c r="I323" s="3" t="n">
+      <c r="I323" s="2" t="n">
         <v>45989</v>
       </c>
       <c r="J323" t="inlineStr">
@@ -17602,7 +17602,7 @@
       <c r="H324" t="n">
         <v>32844897</v>
       </c>
-      <c r="I324" s="3" t="n">
+      <c r="I324" s="2" t="n">
         <v>45992</v>
       </c>
       <c r="J324" t="inlineStr">
@@ -17655,7 +17655,7 @@
       <c r="H325" t="n">
         <v>40878231</v>
       </c>
-      <c r="I325" s="3" t="n">
+      <c r="I325" s="2" t="n">
         <v>45993</v>
       </c>
       <c r="J325" t="inlineStr">
@@ -17708,7 +17708,7 @@
       <c r="H326" t="n">
         <v>42630049</v>
       </c>
-      <c r="I326" s="3" t="n">
+      <c r="I326" s="2" t="n">
         <v>45994</v>
       </c>
       <c r="J326" t="inlineStr">
@@ -17761,7 +17761,7 @@
       <c r="H327" t="n">
         <v>76490308</v>
       </c>
-      <c r="I327" s="3" t="n">
+      <c r="I327" s="2" t="n">
         <v>45995</v>
       </c>
       <c r="J327" t="inlineStr">
@@ -17814,7 +17814,7 @@
       <c r="H328" t="n">
         <v>60754257</v>
       </c>
-      <c r="I328" s="3" t="n">
+      <c r="I328" s="2" t="n">
         <v>45996</v>
       </c>
       <c r="J328" t="inlineStr">
@@ -17867,7 +17867,7 @@
       <c r="H329" t="n">
         <v>97171773</v>
       </c>
-      <c r="I329" s="3" t="n">
+      <c r="I329" s="2" t="n">
         <v>45999</v>
       </c>
       <c r="J329" t="inlineStr">
@@ -17920,7 +17920,7 @@
       <c r="H330" t="n">
         <v>64458336</v>
       </c>
-      <c r="I330" s="3" t="n">
+      <c r="I330" s="2" t="n">
         <v>46000</v>
       </c>
       <c r="J330" t="inlineStr">
@@ -17973,7 +17973,7 @@
       <c r="H331" t="n">
         <v>58620301</v>
       </c>
-      <c r="I331" s="3" t="n">
+      <c r="I331" s="2" t="n">
         <v>46001</v>
       </c>
       <c r="J331" t="inlineStr">
@@ -18026,7 +18026,7 @@
       <c r="H332" t="n">
         <v>52709057</v>
       </c>
-      <c r="I332" s="3" t="n">
+      <c r="I332" s="2" t="n">
         <v>46002</v>
       </c>
       <c r="J332" t="inlineStr">
@@ -18079,7 +18079,7 @@
       <c r="H333" t="n">
         <v>42121847</v>
       </c>
-      <c r="I333" s="3" t="n">
+      <c r="I333" s="2" t="n">
         <v>46003</v>
       </c>
       <c r="J333" t="inlineStr">
@@ -18132,7 +18132,7 @@
       <c r="H334" t="n">
         <v>29717787</v>
       </c>
-      <c r="I334" s="3" t="n">
+      <c r="I334" s="2" t="n">
         <v>46006</v>
       </c>
       <c r="J334" t="inlineStr">
@@ -18185,7 +18185,7 @@
       <c r="H335" t="n">
         <v>33560318</v>
       </c>
-      <c r="I335" s="3" t="n">
+      <c r="I335" s="2" t="n">
         <v>46007</v>
       </c>
       <c r="J335" t="inlineStr">
@@ -18238,7 +18238,7 @@
       <c r="H336" t="n">
         <v>30132656</v>
       </c>
-      <c r="I336" s="3" t="n">
+      <c r="I336" s="2" t="n">
         <v>46008</v>
       </c>
       <c r="J336" t="inlineStr">
@@ -18291,7 +18291,7 @@
       <c r="H337" t="n">
         <v>30665356</v>
       </c>
-      <c r="I337" s="3" t="n">
+      <c r="I337" s="2" t="n">
         <v>46009</v>
       </c>
       <c r="J337" t="inlineStr">
@@ -18344,7 +18344,7 @@
       <c r="H338" t="n">
         <v>36867471</v>
       </c>
-      <c r="I338" s="3" t="n">
+      <c r="I338" s="2" t="n">
         <v>46010</v>
       </c>
       <c r="J338" t="inlineStr">
@@ -18397,7 +18397,7 @@
       <c r="H339" t="n">
         <v>38597474</v>
       </c>
-      <c r="I339" s="3" t="n">
+      <c r="I339" s="2" t="n">
         <v>46013</v>
       </c>
       <c r="J339" t="inlineStr">
@@ -18450,7 +18450,7 @@
       <c r="H340" t="n">
         <v>30065043</v>
       </c>
-      <c r="I340" s="3" t="n">
+      <c r="I340" s="2" t="n">
         <v>46014</v>
       </c>
       <c r="J340" t="inlineStr">
@@ -18503,7 +18503,7 @@
       <c r="H341" t="n">
         <v>43944781</v>
       </c>
-      <c r="I341" s="3" t="n">
+      <c r="I341" s="2" t="n">
         <v>46015</v>
       </c>
       <c r="J341" t="inlineStr">
@@ -18556,7 +18556,7 @@
       <c r="H342" t="n">
         <v>41621396</v>
       </c>
-      <c r="I342" s="3" t="n">
+      <c r="I342" s="2" t="n">
         <v>46017</v>
       </c>
       <c r="J342" t="inlineStr">
@@ -18609,7 +18609,7 @@
       <c r="H343" t="n">
         <v>35151326</v>
       </c>
-      <c r="I343" s="3" t="n">
+      <c r="I343" s="2" t="n">
         <v>46020</v>
       </c>
       <c r="J343" t="inlineStr">
@@ -18662,7 +18662,7 @@
       <c r="H344" t="n">
         <v>101170403</v>
       </c>
-      <c r="I344" s="3" t="n">
+      <c r="I344" s="2" t="n">
         <v>46021</v>
       </c>
       <c r="J344" t="inlineStr">
@@ -18715,7 +18715,7 @@
       <c r="H345" t="n">
         <v>38481459</v>
       </c>
-      <c r="I345" s="3" t="n">
+      <c r="I345" s="2" t="n">
         <v>46022</v>
       </c>
       <c r="J345" t="inlineStr">
@@ -18768,7 +18768,7 @@
       <c r="H346" t="n">
         <v>26668801</v>
       </c>
-      <c r="I346" s="3" t="n">
+      <c r="I346" s="2" t="n">
         <v>46023</v>
       </c>
       <c r="J346" t="inlineStr">
@@ -18821,7 +18821,7 @@
       <c r="H347" t="n">
         <v>59403612</v>
       </c>
-      <c r="I347" s="3" t="n">
+      <c r="I347" s="2" t="n">
         <v>46024</v>
       </c>
       <c r="J347" t="inlineStr">
@@ -18874,7 +18874,7 @@
       <c r="H348" t="n">
         <v>40235429</v>
       </c>
-      <c r="I348" s="3" t="n">
+      <c r="I348" s="2" t="n">
         <v>46027</v>
       </c>
       <c r="J348" t="inlineStr">
@@ -18927,7 +18927,7 @@
       <c r="H349" t="n">
         <v>30967581</v>
       </c>
-      <c r="I349" s="3" t="n">
+      <c r="I349" s="2" t="n">
         <v>46028</v>
       </c>
       <c r="J349" t="inlineStr">
@@ -18980,7 +18980,7 @@
       <c r="H350" t="n">
         <v>48626552</v>
       </c>
-      <c r="I350" s="3" t="n">
+      <c r="I350" s="2" t="n">
         <v>46029</v>
       </c>
       <c r="J350" t="inlineStr">
@@ -19033,7 +19033,7 @@
       <c r="H351" t="n">
         <v>59152770</v>
       </c>
-      <c r="I351" s="3" t="n">
+      <c r="I351" s="2" t="n">
         <v>46030</v>
       </c>
       <c r="J351" t="inlineStr">
@@ -19086,7 +19086,7 @@
       <c r="H352" t="n">
         <v>89479452</v>
       </c>
-      <c r="I352" s="3" t="n">
+      <c r="I352" s="2" t="n">
         <v>46031</v>
       </c>
       <c r="J352" t="inlineStr">
@@ -19139,7 +19139,7 @@
       <c r="H353" t="n">
         <v>66205825</v>
       </c>
-      <c r="I353" s="3" t="n">
+      <c r="I353" s="2" t="n">
         <v>46034</v>
       </c>
       <c r="J353" t="inlineStr">
@@ -19192,7 +19192,7 @@
       <c r="H354" t="n">
         <v>75113220</v>
       </c>
-      <c r="I354" s="3" t="n">
+      <c r="I354" s="2" t="n">
         <v>46035</v>
       </c>
       <c r="J354" t="inlineStr">
@@ -19245,7 +19245,7 @@
       <c r="H355" t="n">
         <v>55680361</v>
       </c>
-      <c r="I355" s="3" t="n">
+      <c r="I355" s="2" t="n">
         <v>46036</v>
       </c>
       <c r="J355" t="inlineStr">
@@ -19298,7 +19298,7 @@
       <c r="H356" t="n">
         <v>104808951</v>
       </c>
-      <c r="I356" s="3" t="n">
+      <c r="I356" s="2" t="n">
         <v>46038</v>
       </c>
       <c r="J356" t="inlineStr">
@@ -19351,7 +19351,7 @@
       <c r="H357" t="n">
         <v>52447662</v>
       </c>
-      <c r="I357" s="3" t="n">
+      <c r="I357" s="2" t="n">
         <v>46041</v>
       </c>
       <c r="J357" t="inlineStr">
@@ -19404,7 +19404,7 @@
       <c r="H358" t="n">
         <v>60720060</v>
       </c>
-      <c r="I358" s="3" t="n">
+      <c r="I358" s="2" t="n">
         <v>46042</v>
       </c>
       <c r="J358" t="inlineStr">
@@ -19457,7 +19457,7 @@
       <c r="H359" t="n">
         <v>77641902</v>
       </c>
-      <c r="I359" s="3" t="n">
+      <c r="I359" s="2" t="n">
         <v>46043</v>
       </c>
       <c r="J359" t="inlineStr">
@@ -19510,7 +19510,7 @@
       <c r="H360" t="n">
         <v>55787837</v>
       </c>
-      <c r="I360" s="3" t="n">
+      <c r="I360" s="2" t="n">
         <v>46044</v>
       </c>
       <c r="J360" t="inlineStr">
@@ -19563,7 +19563,7 @@
       <c r="H361" t="n">
         <v>49017836</v>
       </c>
-      <c r="I361" s="3" t="n">
+      <c r="I361" s="2" t="n">
         <v>46045</v>
       </c>
       <c r="J361" t="inlineStr">
@@ -19582,6 +19582,218 @@
         </is>
       </c>
       <c r="M361" t="inlineStr">
+        <is>
+          <t>BREEZE</t>
+        </is>
+      </c>
+    </row>
+    <row r="362">
+      <c r="A362" t="n">
+        <v>45.79</v>
+      </c>
+      <c r="B362" s="2" t="n">
+        <v>46049</v>
+      </c>
+      <c r="C362" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="D362" t="n">
+        <v>46.25</v>
+      </c>
+      <c r="E362" t="n">
+        <v>44.88</v>
+      </c>
+      <c r="F362" t="n">
+        <v>45.84</v>
+      </c>
+      <c r="G362" t="inlineStr">
+        <is>
+          <t>SUZENE</t>
+        </is>
+      </c>
+      <c r="H362" t="n">
+        <v>62382536</v>
+      </c>
+      <c r="I362" s="3" t="n">
+        <v>46049</v>
+      </c>
+      <c r="J362" t="inlineStr">
+        <is>
+          <t>INE040H01021</t>
+        </is>
+      </c>
+      <c r="K362" t="inlineStr">
+        <is>
+          <t>Suzlon Engergy Ltd</t>
+        </is>
+      </c>
+      <c r="L362" t="inlineStr">
+        <is>
+          <t>SUZENE</t>
+        </is>
+      </c>
+      <c r="M362" t="inlineStr">
+        <is>
+          <t>BREEZE</t>
+        </is>
+      </c>
+    </row>
+    <row r="363">
+      <c r="A363" t="n">
+        <v>47.8</v>
+      </c>
+      <c r="B363" s="2" t="n">
+        <v>46050</v>
+      </c>
+      <c r="C363" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="D363" t="n">
+        <v>48</v>
+      </c>
+      <c r="E363" t="n">
+        <v>46.15</v>
+      </c>
+      <c r="F363" t="n">
+        <v>46.15</v>
+      </c>
+      <c r="G363" t="inlineStr">
+        <is>
+          <t>SUZENE</t>
+        </is>
+      </c>
+      <c r="H363" t="n">
+        <v>59757766</v>
+      </c>
+      <c r="I363" s="3" t="n">
+        <v>46050</v>
+      </c>
+      <c r="J363" t="inlineStr">
+        <is>
+          <t>INE040H01021</t>
+        </is>
+      </c>
+      <c r="K363" t="inlineStr">
+        <is>
+          <t>Suzlon Engergy Ltd</t>
+        </is>
+      </c>
+      <c r="L363" t="inlineStr">
+        <is>
+          <t>SUZENE</t>
+        </is>
+      </c>
+      <c r="M363" t="inlineStr">
+        <is>
+          <t>BREEZE</t>
+        </is>
+      </c>
+    </row>
+    <row r="364">
+      <c r="A364" t="n">
+        <v>47.44</v>
+      </c>
+      <c r="B364" s="2" t="n">
+        <v>46051</v>
+      </c>
+      <c r="C364" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="D364" t="n">
+        <v>48.03</v>
+      </c>
+      <c r="E364" t="n">
+        <v>46.63</v>
+      </c>
+      <c r="F364" t="n">
+        <v>48.03</v>
+      </c>
+      <c r="G364" t="inlineStr">
+        <is>
+          <t>SUZENE</t>
+        </is>
+      </c>
+      <c r="H364" t="n">
+        <v>54843475</v>
+      </c>
+      <c r="I364" s="3" t="n">
+        <v>46051</v>
+      </c>
+      <c r="J364" t="inlineStr">
+        <is>
+          <t>INE040H01021</t>
+        </is>
+      </c>
+      <c r="K364" t="inlineStr">
+        <is>
+          <t>Suzlon Engergy Ltd</t>
+        </is>
+      </c>
+      <c r="L364" t="inlineStr">
+        <is>
+          <t>SUZENE</t>
+        </is>
+      </c>
+      <c r="M364" t="inlineStr">
+        <is>
+          <t>BREEZE</t>
+        </is>
+      </c>
+    </row>
+    <row r="365">
+      <c r="A365" t="n">
+        <v>47.67</v>
+      </c>
+      <c r="B365" s="2" t="n">
+        <v>46052</v>
+      </c>
+      <c r="C365" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="D365" t="n">
+        <v>47.95</v>
+      </c>
+      <c r="E365" t="n">
+        <v>46.81</v>
+      </c>
+      <c r="F365" t="n">
+        <v>47.4</v>
+      </c>
+      <c r="G365" t="inlineStr">
+        <is>
+          <t>SUZENE</t>
+        </is>
+      </c>
+      <c r="H365" t="n">
+        <v>60470060</v>
+      </c>
+      <c r="I365" s="3" t="n">
+        <v>46052</v>
+      </c>
+      <c r="J365" t="inlineStr">
+        <is>
+          <t>INE040H01021</t>
+        </is>
+      </c>
+      <c r="K365" t="inlineStr">
+        <is>
+          <t>Suzlon Engergy Ltd</t>
+        </is>
+      </c>
+      <c r="L365" t="inlineStr">
+        <is>
+          <t>SUZENE</t>
+        </is>
+      </c>
+      <c r="M365" t="inlineStr">
         <is>
           <t>BREEZE</t>
         </is>

</xml_diff>